<commit_message>
paraphrased for len(ops) > 2
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/stratified_test.xlsx
+++ b/textToOps/data/processed/stratified_test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,24 +552,28 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What are the land use inside the flood zones in Oleander</t>
+          <t>How many luxury hotels are in Happy Valley ski resort</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Happy Valley ski resort</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>tourism=hotel, stars=*</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>done</t>
@@ -580,16 +584,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
@@ -602,11 +598,11 @@
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="W2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X2" t="b">
         <v>0</v>
@@ -614,26 +610,30 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What areas are not park in Houston</t>
+          <t>What area are within 50 km from family physician services in Saskatchewan</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Houston</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>Saskatchewan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>leisure=park</t>
+          <t>amenity=doctor</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -646,8 +646,16 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
@@ -660,11 +668,11 @@
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="W3" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="X3" t="b">
         <v>0</v>
@@ -672,26 +680,26 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B4" t="n">
         <v>15</v>
       </c>
-      <c r="B4" t="n">
-        <v>24</v>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>What areas are outside 155 meters from nature reserve districts in Houston</t>
+          <t>What areas are inside 1000 foot of schools in El Cajon</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>El Cajon</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>leisure=nature_reserve</t>
+          <t>amenity=school, amenity=kindergarten</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -738,14 +746,14 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>What areas are outside 300 meters from streams in Houston</t>
+          <t>What areas are outside 150 meters from hospitals in Houston</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -757,7 +765,7 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>waterway=stream</t>
+          <t>amenity=hospital</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -804,26 +812,26 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>What areas are outside 5000 meters of the roads in Spain</t>
+          <t>What areas are outside 60 meters from water body in Houston</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>highway=*</t>
+          <t>landuse=aquaculture, basin, salt_pond</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -870,26 +878,30 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>What areas are within 300 meters of runways in Schiphol airport</t>
+          <t xml:space="preserve">What areas are within 1000 meters of roads in Assam </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Schiphol airport</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>Assam</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>aeroway=runway</t>
+          <t>highway=*</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -939,23 +951,23 @@
         <v>34</v>
       </c>
       <c r="B8" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>What areas are within 500 meters from religious places in Karbala in Iraq</t>
+          <t>What areas are within 1000 meters of the schools in Oleander</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Karbala, Iraq</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>landuse=religious</t>
+          <t>amenity=school</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1002,28 +1014,24 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B9" t="n">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>What areas are within 60 minutes of airports in Crook, Deschutes, and Jefferson county</t>
+          <t>What areas do have altitude between 700 and 2000 meters in Spain</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Crook, Deschutes, Jefferson county</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> aeroway=*</t>
-        </is>
-      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>done</t>
@@ -1031,22 +1039,22 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Topography</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>classification</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Data model conversion</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1064,11 +1072,11 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="X9" t="b">
         <v>0</v>
@@ -1076,28 +1084,24 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="B10" t="n">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>What areas are within a quarter mile of a store in Gresham</t>
+          <t>What is the average rating of street pavement for each borough in New York City</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Gresham</t>
+          <t>New York City</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>shop=*</t>
-        </is>
-      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>done</t>
@@ -1105,20 +1109,24 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Data editing</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr"/>
+          <t>Data editing</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -1130,11 +1138,11 @@
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data editing,overlay analysis,data editing,data queries</t>
         </is>
       </c>
       <c r="W10" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="X10" t="b">
         <v>0</v>
@@ -1142,23 +1150,27 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B11" t="n">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>What areas do have slope larger than 10 percent in Spain</t>
+          <t>What is the cervix cancer mortality rate of white females for each city in the Western USA from 1970 to 1994</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t xml:space="preserve">the Western USA </t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>from 1970 to 1994</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
@@ -1167,29 +1179,17 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Topography</t>
+          <t>Data editing</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
@@ -1200,11 +1200,11 @@
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr">
         <is>
-          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="W11" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="X11" t="b">
         <v>0</v>
@@ -1212,26 +1212,26 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B12" t="n">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>What is the density surface of rainfall measurements in the Netherlands</t>
+          <t>What is the Euclidean distance to recreational sites in Utrecht</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>the Netherlands</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> man_made=monitoring_station</t>
+          <t>landuse=recreation_ground</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1274,28 +1274,24 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B13" t="n">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>What is the density surface of temperature measurements in Oleander city</t>
+          <t>What is the Euclidean distance to subway stations in Amsterdam</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Oleander city</t>
+          <t>Amsterdam</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> man_made=monitoring_station</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>done</t>
@@ -1336,26 +1332,22 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B14" t="n">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>What is the kernel density of crime in Surrey in UK</t>
+          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Surrey</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>UK</t>
-        </is>
-      </c>
+          <t>Oleander city</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
@@ -1398,28 +1390,24 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="B15" t="n">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>What is the land use in Netherlands</t>
+          <t>What is the mean center of the fire calls weighted by the priority in Fort Worth</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Fort Worth</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>landuse=*</t>
-        </is>
-      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>done</t>
@@ -1430,8 +1418,16 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
@@ -1444,11 +1440,11 @@
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
         </is>
       </c>
       <c r="W15" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="X15" t="b">
         <v>0</v>
@@ -1456,26 +1452,26 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B16" t="n">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Where are the industrial areas in Utrecht</t>
+          <t>What liquor stores are within 1000 foot of libraries in El Cajon</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>El Cajon</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>landuse=industrial</t>
+          <t>shop=alcohol, amenity=library</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1490,15 +1486,19 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
+          <t>buffer</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr"/>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
@@ -1510,11 +1510,11 @@
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="W16" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="X16" t="b">
         <v>0</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="B17" t="n">
         <v>121</v>
@@ -1588,26 +1588,26 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="B18" t="n">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Which houses are for sale in Utrecht</t>
+          <t>Where are the ski pistes in Happy Valley ski resort</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Happy Valley ski resort</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>building=house</t>
+          <t>site=piste</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1617,15 +1617,19 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr"/>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
@@ -1638,11 +1642,11 @@
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t>data queries,geometry measurement,data queries</t>
         </is>
       </c>
       <c r="W18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X18" t="b">
         <v>0</v>
@@ -1650,26 +1654,26 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B19" t="n">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Which vacant lots are within 1 mile of a freeway in Hillsboro</t>
+          <t>Which houses are within 2 minutes driving time from fire stations  (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Hillsboro</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>abandoned:*=*, highway=motorway</t>
+          <t>amenity=fire_station</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1684,20 +1688,24 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
@@ -1708,13 +1716,203 @@
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="W19" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="X19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B20" t="n">
+        <v>127</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Which houses have construction year between 1990 and 2000 in Utrecht</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>year_of_construction=*</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>data queries</t>
+        </is>
+      </c>
+      <c r="W20" t="n">
+        <v>1</v>
+      </c>
+      <c r="X20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B21" t="n">
+        <v>128</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Which land use contains meteorological stations in Netherlands</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> man_made=monitoring_station</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>data queries,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="W21" t="n">
+        <v>2</v>
+      </c>
+      <c r="X21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B22" t="n">
+        <v>135</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Which wind farm proposals are nearest to the roads in Scotland</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>highway=*</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>network analysis</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>data queries,network analysis,data queries</t>
+        </is>
+      </c>
+      <c r="W22" t="n">
+        <v>4</v>
+      </c>
+      <c r="X22" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit for curl unique data
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/stratified_test.xlsx
+++ b/textToOps/data/processed/stratified_test.xlsx
@@ -552,26 +552,26 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>How many luxury hotels are in Happy Valley ski resort</t>
+          <t>What areas are inside 1000 foot of schools in El Cajon</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Happy Valley ski resort</t>
+          <t>El Cajon</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>tourism=hotel, stars=*</t>
+          <t>amenity=school, amenity=kindergarten</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -584,8 +584,16 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
@@ -598,11 +606,11 @@
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="W2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="X2" t="b">
         <v>0</v>
@@ -610,30 +618,26 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What area are within 50 km from family physician services in Saskatchewan</t>
+          <t>What areas are not park in Houston</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Saskatchewan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>amenity=doctor</t>
+          <t>leisure=park</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -646,16 +650,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Buffer</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
@@ -668,11 +664,11 @@
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="W3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="X3" t="b">
         <v>0</v>
@@ -680,26 +676,26 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>What areas are inside 1000 foot of schools in El Cajon</t>
+          <t>What areas are outside 250 meters of human settlement in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>El Cajon</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>amenity=school, amenity=kindergarten</t>
+          <t>residential=*</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -746,26 +742,26 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>What areas are outside 150 meters from hospitals in Houston</t>
+          <t>What areas are outside 3000 meters of the rivers in Spain</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>amenity=hospital</t>
+          <t>waterway=river</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -812,26 +808,26 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>What areas are outside 60 meters from water body in Houston</t>
+          <t>What areas are within 10 miles of current transmission lines with a voltage greater than 400 in Colorado</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>landuse=aquaculture, basin, salt_pond</t>
+          <t>power=line</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -948,26 +944,26 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B8" t="n">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>What areas are within 1000 meters of the schools in Oleander</t>
+          <t>What areas are within 60 minutes of airports in Crook, Deschutes, and Jefferson county</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Crook, Deschutes, Jefferson county</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>amenity=school</t>
+          <t xml:space="preserve"> aeroway=*</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -982,16 +978,24 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
@@ -1002,11 +1006,11 @@
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="W8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="X8" t="b">
         <v>0</v>
@@ -1014,24 +1018,28 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B9" t="n">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>What areas do have altitude between 700 and 2000 meters in Spain</t>
+          <t>What areas are within a quarter mile of light rail stop in Gresham</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Gresham</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>railway=tram_stop, light_rail</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>done</t>
@@ -1039,29 +1047,21 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Topography</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
@@ -1072,11 +1072,11 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr">
         <is>
-          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="W9" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="X9" t="b">
         <v>0</v>
@@ -1084,19 +1084,19 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B10" t="n">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>What is the average rating of street pavement for each borough in New York City</t>
+          <t>What areas have an aspect larger than 45 degree and smaller than 135 degrees in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>New York City</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -1109,25 +1109,29 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Data editing</t>
+          <t>Topography</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Data editing</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
@@ -1138,11 +1142,11 @@
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data editing,data queries</t>
+          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="W10" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="X10" t="b">
         <v>0</v>
@@ -1150,28 +1154,28 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B11" t="n">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>What is the cervix cancer mortality rate of white females for each city in the Western USA from 1970 to 1994</t>
+          <t>What houses are for sale in urban areas in Utrecht</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">the Western USA </t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>from 1970 to 1994</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>boundary=urban, building=house</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t>done</t>
@@ -1179,15 +1183,19 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr"/>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
@@ -1200,11 +1208,11 @@
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t>data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="W11" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="X11" t="b">
         <v>0</v>
@@ -1212,26 +1220,26 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B12" t="n">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to recreational sites in Utrecht</t>
+          <t>What is the density surface of temperature measurements in Oleander city</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Oleander city</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>landuse=recreation_ground</t>
+          <t xml:space="preserve"> man_made=monitoring_station</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1274,19 +1282,19 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B13" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to subway stations in Amsterdam</t>
+          <t>What is the Euclidean distance to the rivers in Crook, Deschutes, and Jefferson county</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Amsterdam</t>
+          <t>Crook, Deschutes, Jefferson county</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -1332,23 +1340,27 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B14" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
+          <t>What is the lung cancer mortality rate of white males for each city in the Western USA from 1970 to 1994</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Oleander city</t>
+          <t>the Western USA</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> from 1970 to 1994</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
@@ -1357,12 +1369,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
@@ -1378,11 +1390,11 @@
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="W14" t="n">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="X14" t="b">
         <v>0</v>
@@ -1390,19 +1402,19 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B15" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>What is the mean center of the fire calls weighted by the priority in Fort Worth</t>
+          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Fort Worth</t>
+          <t>Oleander city</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -1420,14 +1432,10 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
           <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
@@ -1440,11 +1448,11 @@
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="W15" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="X15" t="b">
         <v>0</v>
@@ -1452,28 +1460,24 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B16" t="n">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>What liquor stores are within 1000 foot of libraries in El Cajon</t>
+          <t>What is the mean center of the fire calls weighted by the priority in Fort Worth</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>El Cajon</t>
+          <t>Fort Worth</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>shop=alcohol, amenity=library</t>
-        </is>
-      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>done</t>
@@ -1486,19 +1490,15 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>buffer</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
@@ -1510,11 +1510,11 @@
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries</t>
+          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
         </is>
       </c>
       <c r="W16" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="X16" t="b">
         <v>0</v>
@@ -1522,28 +1522,28 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B17" t="n">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Where are the rocky areas in Spain</t>
+          <t>What is the median people age for each census tract in Tarrant County</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>Tarrant County</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Texas</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>nature : bare_rock</t>
-        </is>
-      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>done</t>
@@ -1551,20 +1551,24 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr"/>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
@@ -1576,11 +1580,11 @@
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data editing,overlay analysis,data editing,data queries</t>
         </is>
       </c>
       <c r="W17" t="n">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="X17" t="b">
         <v>0</v>
@@ -1588,26 +1592,26 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B18" t="n">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Where are the ski pistes in Happy Valley ski resort</t>
+          <t>Where are not conservation areas in UK</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Happy Valley ski resort</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>site=piste</t>
+          <t>landuse=conservation</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1654,26 +1658,26 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B19" t="n">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Which houses are within 2 minutes driving time from fire stations  (from my current location) in Oleander</t>
+          <t>Where are the industrial areas in Utrecht</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>amenity=fire_station</t>
+          <t>landuse=industrial</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1688,24 +1692,16 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Geometry measurement</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
@@ -1716,11 +1712,11 @@
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>data queries,geometry measurement,data queries</t>
         </is>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X19" t="b">
         <v>0</v>
@@ -1728,26 +1724,26 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B20" t="n">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Which houses have construction year between 1990 and 2000 in Utrecht</t>
+          <t>Which shops are open at 6 pm in Happy Valley ski resort</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Happy Valley ski resort</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>year_of_construction=*</t>
+          <t>opening_hours=*</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1786,26 +1782,26 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B21" t="n">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Which land use contains meteorological stations in Netherlands</t>
+          <t>Which vacant lots are within 1 mile of a freeway in Hillsboro</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Hillsboro</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> man_made=monitoring_station</t>
+          <t>abandoned:*=*, highway=motorway</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1820,15 +1816,19 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr"/>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
@@ -1840,11 +1840,11 @@
       <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries</t>
+          <t>data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="W21" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="X21" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Changed data with ignore index
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/stratified_test.xlsx
+++ b/textToOps/data/processed/stratified_test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA28"/>
+  <dimension ref="A1:AA41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,28 +567,24 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What areas are inside 1000 foot of schools in El Cajon</t>
+          <t>What are the areas within a four-minute drive of each fire station at 2 a.m. on Tuesday in Utrecht</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>El Cajon</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>amenity=school, amenity=kindergarten</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>done</t>
@@ -601,16 +597,24 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>network analysis</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
@@ -624,11 +628,11 @@
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="b">
         <v>0</v>
@@ -636,24 +640,32 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What areas are not conatined as green belt areas in Houston</t>
+          <t>What area are within 50 km from family physician services in Saskatchewan in Canada</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Houston</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>Saskatchewan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>amenity=doctor</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>done</t>
@@ -666,10 +678,14 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
@@ -685,11 +701,11 @@
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z3" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AA3" t="b">
         <v>0</v>
@@ -697,26 +713,26 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>What areas are not park in Houston</t>
+          <t>What areas are inside 1000 foot of schools in El Cajon</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>El Cajon</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>leisure=park</t>
+          <t>amenity=school, amenity=kindergarten</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -729,8 +745,16 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
@@ -746,11 +770,11 @@
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AA4" t="b">
         <v>0</v>
@@ -758,28 +782,24 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>What areas are outside 250 meters of human settlement in the Cape Peninsula</t>
+          <t>What areas are green belt areas in Houston</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>residential=*</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>done</t>
@@ -792,14 +812,10 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Buffer</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
@@ -815,11 +831,11 @@
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z5" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AA5" t="b">
         <v>0</v>
@@ -827,28 +843,24 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B6" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>What areas are outside 3000 meters of the rivers in Spain</t>
+          <t>What areas are not conatined as green belt areas in Houston</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>waterway=river</t>
-        </is>
-      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>done</t>
@@ -861,14 +873,10 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Buffer</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
@@ -884,11 +892,11 @@
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z6" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AA6" t="b">
         <v>0</v>
@@ -896,26 +904,26 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B7" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>What areas are within 10 miles of current transmission lines with a voltage greater than 400 in Colorado</t>
+          <t>What areas are not park in Houston</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>power=line</t>
+          <t>leisure=park</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -928,16 +936,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Buffer</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
@@ -953,11 +953,11 @@
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="Z7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AA7" t="b">
         <v>0</v>
@@ -965,26 +965,26 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B8" t="n">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>What areas are within 2000 meters of the playgrounds in Oleander</t>
+          <t>What areas are not wetlands in Houston</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>leisure=playground</t>
+          <t>natural=wetland</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -997,16 +997,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Buffer</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
@@ -1022,11 +1014,11 @@
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="Z8" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AA8" t="b">
         <v>0</v>
@@ -1034,24 +1026,28 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>What areas are within 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
+          <t>What areas are outside 250 meters of human settlement in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>residential=*</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>done</t>
@@ -1064,34 +1060,18 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Network analysis</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
@@ -1099,19 +1079,15 @@
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>어디로 부터 가장 가까운 소방서</t>
-        </is>
-      </c>
+      <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis,어디로 부터 가장 가까운 소방서</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z9" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AA9" t="b">
         <v>0</v>
@@ -1119,26 +1095,26 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B10" t="n">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>What areas are within 60 minutes of airports in Crook, Deschutes, and Jefferson county</t>
+          <t>What areas are outside 3000 meters of the rivers in Spain</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Crook, Deschutes, Jefferson county</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> aeroway=*</t>
+          <t>waterway=river</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1153,24 +1129,16 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
@@ -1184,11 +1152,11 @@
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA10" t="b">
         <v>0</v>
@@ -1196,24 +1164,28 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>What areas have an annual rainfall of more than 1000 millimeters in the Cape Peninsula</t>
+          <t>What areas are within 10 miles of current transmission lines with a voltage greater than 400 in Colorado</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>power=line</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t>done</t>
@@ -1221,29 +1193,21 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
@@ -1257,11 +1221,11 @@
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z11" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="AA11" t="b">
         <v>0</v>
@@ -1269,24 +1233,28 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B12" t="n">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>What areas have an aspect larger than 45 degree and smaller than 135 degrees in the Cape Peninsula</t>
+          <t>What areas are within 2000 meters of the playgrounds in Oleander</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>leisure=playground</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
           <t>done</t>
@@ -1294,29 +1262,21 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Topography</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
@@ -1330,11 +1290,11 @@
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z12" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AA12" t="b">
         <v>0</v>
@@ -1342,28 +1302,24 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="B13" t="n">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>What houses are for sale and within 1km from the nearest school (from my current location) in Utrecht</t>
+          <t>What areas are within 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>amenity=school, building=house</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>done</t>
@@ -1371,31 +1327,39 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>buffer</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
@@ -1403,15 +1367,19 @@
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>어디로 부터 가장 가까운 소방서</t>
+        </is>
+      </c>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
+          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis,어디로 부터 가장 가까운 소방서</t>
         </is>
       </c>
       <c r="Z13" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="AA13" t="b">
         <v>0</v>
@@ -1419,26 +1387,26 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B14" t="n">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>What houses are greather than 30 square meters in urban areas in Utrecht</t>
+          <t>What areas are within 60 minutes of airports in Crook, Deschutes, and Jefferson county</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Crook, Deschutes, Jefferson county</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>boundary=urban, building=house</t>
+          <t xml:space="preserve"> aeroway=*</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1453,16 +1421,24 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
@@ -1472,19 +1448,15 @@
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
-        </is>
-      </c>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries,osm urban이 있긴 하지만 거의 안쓴다</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z14" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AA14" t="b">
         <v>0</v>
@@ -1492,26 +1464,30 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B15" t="n">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>What is the central feature of bank branches in Oleander</t>
+          <t>What areas are within one mile of main roads in Loudoun County in US</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Oleander</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
+          <t>Loudoun County</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>amenity=bank</t>
+          <t>highway=motorway</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1526,12 +1502,12 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Generalization</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="L15" t="inlineStr"/>
@@ -1544,20 +1520,16 @@
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr">
-        <is>
-          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
-        </is>
-      </c>
+      <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>data queries,generalization,geostatistics  ,https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z15" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="AA15" t="b">
         <v>0</v>
@@ -1565,28 +1537,24 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="B16" t="n">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>What is the density surface of temperature measurements in Oleander city</t>
+          <t>What areas have an annual amount of snowfall more than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Oleander city</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> man_made=monitoring_station</t>
-        </is>
-      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>done</t>
@@ -1594,17 +1562,29 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
@@ -1618,11 +1598,11 @@
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z16" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="AA16" t="b">
         <v>0</v>
@@ -1630,19 +1610,19 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="B17" t="n">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to the rivers in Crook, Deschutes, and Jefferson county</t>
+          <t>What areas have an annual rainfall of more than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Crook, Deschutes, Jefferson county</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -1655,17 +1635,29 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
@@ -1679,11 +1671,11 @@
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z17" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="AA17" t="b">
         <v>0</v>
@@ -1691,19 +1683,19 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="B18" t="n">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
+          <t>What areas have an aspect larger than 45 degree and smaller than 135 degrees in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Oleander city</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1716,17 +1708,29 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Topography</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
@@ -1740,11 +1744,11 @@
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z18" t="n">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="AA18" t="b">
         <v>0</v>
@@ -1752,24 +1756,28 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="B19" t="n">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>What is the mean center of the fire calls weighted by the priority in Fort Worth</t>
+          <t>What houses are larger than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Fort Worth</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>amenity=school, building=house</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr">
         <is>
           <t>done</t>
@@ -1777,21 +1785,29 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>network analysis</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
@@ -1805,11 +1821,11 @@
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z19" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="AA19" t="b">
         <v>0</v>
@@ -1817,28 +1833,28 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="B20" t="n">
-        <v>139</v>
+        <v>86</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>What is the median household income for each census block in Tarrant County in Texas</t>
+          <t>What houses are for sale and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Tarrant County</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Texas</t>
-        </is>
-      </c>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>amenity=school, building=house</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
           <t>done</t>
@@ -1846,25 +1862,29 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>network analysis</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>data editing</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr"/>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
@@ -1878,11 +1898,11 @@
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data editing,data queries</t>
+          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z20" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="AA20" t="b">
         <v>0</v>
@@ -1890,28 +1910,28 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="B21" t="n">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>What is the median people age for each census tract in Tarrant County in Texas</t>
+          <t>What houses are for sale in flood zone in Utrecht</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Tarrant County</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Texas</t>
-        </is>
-      </c>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>boundary=urban, building=house</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr">
         <is>
           <t>done</t>
@@ -1919,7 +1939,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1929,14 +1949,10 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>data editing</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
@@ -1947,15 +1963,19 @@
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr"/>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
+        </is>
+      </c>
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data editing,data queries</t>
+          <t>data queries,overlay analysis,data queries,osm urban이 있긴 하지만 거의 안쓴다</t>
         </is>
       </c>
       <c r="Z21" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AA21" t="b">
         <v>0</v>
@@ -1963,30 +1983,26 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="B22" t="n">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Where are not protected region in Assam in India</t>
+          <t>What houses are greather than 30 square meters in urban areas in Utrecht</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>landuse=conservation</t>
+          <t>boundary=urban, building=house</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -2001,7 +2017,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2020,15 +2036,19 @@
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
-      <c r="W22" t="inlineStr"/>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
+        </is>
+      </c>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data queries,overlay analysis,data queries,osm urban이 있긴 하지만 거의 안쓴다</t>
         </is>
       </c>
       <c r="Z22" t="n">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="AA22" t="b">
         <v>0</v>
@@ -2036,26 +2056,26 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>124</v>
+        <v>79</v>
       </c>
       <c r="B23" t="n">
-        <v>164</v>
+        <v>105</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Where are the rocky areas in Spain</t>
+          <t>What is the central feature of bank branches in Oleander</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>nature : bare_rock</t>
+          <t>amenity=bank</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2070,12 +2090,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
+          <t>Generalization</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="L23" t="inlineStr"/>
@@ -2088,16 +2108,20 @@
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
+        </is>
+      </c>
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data queries,generalization,geostatistics  ,https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
         </is>
       </c>
       <c r="Z23" t="n">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AA23" t="b">
         <v>0</v>
@@ -2105,26 +2129,26 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="B24" t="n">
-        <v>167</v>
+        <v>112</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Which houses are for sale in Utrecht</t>
+          <t>What is the density surface of temperature measurements in Oleander city</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Oleander city</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>building=house</t>
+          <t xml:space="preserve"> man_made=monitoring_station</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2134,12 +2158,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="K24" t="inlineStr"/>
@@ -2158,11 +2182,11 @@
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z24" t="n">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="AA24" t="b">
         <v>0</v>
@@ -2170,28 +2194,24 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="B25" t="n">
-        <v>170</v>
+        <v>115</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Which houses have construction year between 1990 and 2000 in Utrecht</t>
+          <t>What is the Euclidean distance to green areas in Amsterdam</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Amsterdam</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>year_of_construction=*</t>
-        </is>
-      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
           <t>done</t>
@@ -2202,7 +2222,11 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
@@ -2219,11 +2243,11 @@
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z25" t="n">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="AA25" t="b">
         <v>0</v>
@@ -2231,28 +2255,24 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="B26" t="n">
-        <v>177</v>
+        <v>120</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Which schools are not within 3 minutes of driving time from a fire station in Fort Worth</t>
+          <t>What is the Euclidean distance to the rivers in Crook, Deschutes, and Jefferson county</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Fort Worth</t>
+          <t>Crook, Deschutes, Jefferson county</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>amenity=fire_station, amenity=school</t>
-        </is>
-      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
           <t>done</t>
@@ -2265,29 +2285,13 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Network analysis</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
@@ -2300,11 +2304,11 @@
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z26" t="n">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="AA26" t="b">
         <v>0</v>
@@ -2312,28 +2316,28 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="B27" t="n">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Which vacant lots are within 1 mile of a freeway in Hillsboro</t>
+          <t>What is the lung cancer mortality rate of white males for each city in the Western USA from 1970 to 1994</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Hillsboro</t>
+          <t>the Western USA</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>abandoned:*=*, highway=motorway</t>
-        </is>
-      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> from 1970 to 1994</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
           <t>done</t>
@@ -2341,24 +2345,16 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>buffer</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
@@ -2373,11 +2369,11 @@
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries</t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="Z27" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="AA27" t="b">
         <v>0</v>
@@ -2385,28 +2381,24 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="B28" t="n">
-        <v>185</v>
+        <v>129</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Which wind farm proposals are nearest to the roads in Scotland</t>
+          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Scotland</t>
+          <t>Oleander city</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>highway=*</t>
-        </is>
-      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
           <t>done</t>
@@ -2419,14 +2411,10 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>network analysis</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
@@ -2442,13 +2430,926 @@
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr">
         <is>
+          <t xml:space="preserve">data queries,geostatistics  </t>
+        </is>
+      </c>
+      <c r="Z28" t="n">
+        <v>41</v>
+      </c>
+      <c r="AA28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B29" t="n">
+        <v>134</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>What is the mean center of the fire calls weighted by the priority in Fort Worth</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+        </is>
+      </c>
+      <c r="Z29" t="n">
+        <v>44</v>
+      </c>
+      <c r="AA29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B30" t="n">
+        <v>139</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>What is the median household income for each census block in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Texas</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>data editing,overlay analysis,data editing,data queries</t>
+        </is>
+      </c>
+      <c r="Z30" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B31" t="n">
+        <v>141</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>What is the median people age for each census tract in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Texas</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>data editing,overlay analysis,data editing,data queries</t>
+        </is>
+      </c>
+      <c r="Z31" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B32" t="n">
+        <v>149</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>What liquor stores are within 1000 foot of schools in El Cajon</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>El Cajon</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>shop=alcohol, amenity=school</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>data queries,buffer,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z32" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B33" t="n">
+        <v>153</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Where are not protected region in Assam in India</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Assam</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>landuse=conservation</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="Z33" t="n">
+        <v>47</v>
+      </c>
+      <c r="AA33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B34" t="n">
+        <v>156</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Where are the commercial areas in Amsterdam</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Amsterdam</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>landuse=commercial</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="Z34" t="n">
+        <v>47</v>
+      </c>
+      <c r="AA34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B35" t="n">
+        <v>164</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Where are the rocky areas in Spain</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>nature : bare_rock</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
+      <c r="T35" t="inlineStr"/>
+      <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
+      <c r="X35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="Z35" t="n">
+        <v>47</v>
+      </c>
+      <c r="AA35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B36" t="n">
+        <v>167</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Which houses are for sale in Utrecht</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>building=house</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr"/>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
+      <c r="X36" t="inlineStr"/>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>data editing,data queries</t>
+        </is>
+      </c>
+      <c r="Z36" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B37" t="n">
+        <v>170</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Which houses have construction year between 1990 and 2000 in Utrecht</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>year_of_construction=*</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr"/>
+      <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
+      <c r="X37" t="inlineStr"/>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>data queries</t>
+        </is>
+      </c>
+      <c r="Z37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B38" t="n">
+        <v>177</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Which schools are not within 3 minutes of driving time from a fire station in Fort Worth</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>amenity=fire_station, amenity=school</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>data queries</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr"/>
+      <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
+      <c r="X38" t="inlineStr"/>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z38" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B39" t="n">
+        <v>179</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Which vacant lots are within 1 mile of a freeway in Hillsboro</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Hillsboro</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>abandoned:*=*, highway=motorway</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr"/>
+      <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
+      <c r="X39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>data queries,buffer,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z39" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B40" t="n">
+        <v>183</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Which wind farm proposals are nearest to the high way in Scotland</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>highway=*</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>network analysis</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+      <c r="X40" t="inlineStr"/>
+      <c r="Y40" t="inlineStr">
+        <is>
           <t>data queries,network analysis,data queries</t>
         </is>
       </c>
-      <c r="Z28" t="n">
+      <c r="Z40" t="n">
         <v>4</v>
       </c>
-      <c r="AA28" t="b">
+      <c r="AA40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B41" t="n">
+        <v>185</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Which wind farm proposals are nearest to the roads in Scotland</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>highway=*</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>network analysis</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>data queries,network analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z41" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA41" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Paraphrased with more than 2
 Class checked. Test contains at least 1
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/stratified_test.xlsx
+++ b/textToOps/data/processed/stratified_test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA41"/>
+  <dimension ref="A1:AA60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,7 +567,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -643,27 +643,23 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What area are within 50 km from family physician services in Saskatchewan in Canada</t>
+          <t>What are the two fire stations closest to each school in Utrecht</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Saskatchewan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>amenity=doctor</t>
+          <t>amenity=fire_station, amenity=school</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -678,12 +674,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
@@ -701,11 +697,11 @@
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,network analysis,data queries</t>
         </is>
       </c>
       <c r="Z3" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="AA3" t="b">
         <v>0</v>
@@ -716,23 +712,27 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>What areas are inside 1000 foot of schools in El Cajon</t>
+          <t>What area are within 50 km from family physician services in Saskatchewan in Canada</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>El Cajon</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>Saskatchewan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>amenity=school, amenity=kindergarten</t>
+          <t>amenity=doctor</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -782,24 +782,28 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>What areas are green belt areas in Houston</t>
+          <t>What areas are inside 1000 foot of schools in El Cajon</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>El Cajon</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>amenity=school, amenity=kindergarten</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
           <t>done</t>
@@ -812,10 +816,14 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
@@ -831,11 +839,11 @@
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z5" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AA5" t="b">
         <v>0</v>
@@ -843,14 +851,14 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>What areas are not conatined as green belt areas in Houston</t>
+          <t>What areas are green belt areas in Houston</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -907,11 +915,11 @@
         <v>17</v>
       </c>
       <c r="B7" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>What areas are not park in Houston</t>
+          <t>What areas are not conatined as green belt areas in Houston</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -921,11 +929,7 @@
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>leisure=park</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>done</t>
@@ -936,7 +940,11 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
@@ -953,11 +961,11 @@
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t>data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z7" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="AA7" t="b">
         <v>0</v>
@@ -965,14 +973,14 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>What areas are not wetlands in Houston</t>
+          <t>What areas are not park in Houston</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -984,7 +992,7 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>natural=wetland</t>
+          <t>leisure=park</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1026,26 +1034,26 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>What areas are outside 250 meters of human settlement in the Cape Peninsula</t>
+          <t>What areas are not wetlands in Houston</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>residential=*</t>
+          <t>natural=wetland</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1058,16 +1066,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Buffer</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
@@ -1083,11 +1083,11 @@
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="Z9" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AA9" t="b">
         <v>0</v>
@@ -1098,23 +1098,23 @@
         <v>24</v>
       </c>
       <c r="B10" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>What areas are outside 3000 meters of the rivers in Spain</t>
+          <t>What areas are outside 250 meters of human settlement in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>waterway=river</t>
+          <t>residential=*</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1164,26 +1164,26 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>What areas are within 10 miles of current transmission lines with a voltage greater than 400 in Colorado</t>
+          <t>What areas are outside 3000 meters of the rivers in Spain</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>power=line</t>
+          <t>waterway=river</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1233,26 +1233,26 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>What areas are within 2000 meters of the playgrounds in Oleander</t>
+          <t>What areas are within 10 miles of current transmission lines with a voltage greater than 400 in Colorado</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>leisure=playground</t>
+          <t>power=line</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1302,14 +1302,14 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13" t="n">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>What areas are within 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
+          <t>What areas are within 2000 meters of the playgrounds in Oleander</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1319,7 +1319,11 @@
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>leisure=playground</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
           <t>done</t>
@@ -1332,34 +1336,18 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>Network analysis</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
@@ -1367,19 +1355,15 @@
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>어디로 부터 가장 가까운 소방서</t>
-        </is>
-      </c>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis,어디로 부터 가장 가까운 소방서</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z13" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AA13" t="b">
         <v>0</v>
@@ -1387,28 +1371,24 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B14" t="n">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>What areas are within 60 minutes of airports in Crook, Deschutes, and Jefferson county</t>
+          <t>What areas are accessible within 3 minutes of by car from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Crook, Deschutes, Jefferson county</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> aeroway=*</t>
-        </is>
-      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>done</t>
@@ -1426,21 +1406,29 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
           <t>classification</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
@@ -1448,15 +1436,19 @@
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>어디로 부터 가장 가까운 소방서</t>
+        </is>
+      </c>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis,어디로 부터 가장 가까운 소방서</t>
         </is>
       </c>
       <c r="Z14" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AA14" t="b">
         <v>0</v>
@@ -1464,32 +1456,24 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B15" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>What areas are within one mile of main roads in Loudoun County in US</t>
+          <t>What areas are within 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Loudoun County</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
+          <t>Oleander</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>highway=motorway</t>
-        </is>
-      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>done</t>
@@ -1502,18 +1486,34 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
@@ -1521,15 +1521,19 @@
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>어디로 부터 가장 가까운 소방서</t>
+        </is>
+      </c>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis,어디로 부터 가장 가까운 소방서</t>
         </is>
       </c>
       <c r="Z15" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="AA15" t="b">
         <v>0</v>
@@ -1537,24 +1541,28 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B16" t="n">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>What areas have an annual amount of snowfall more than 1000 millimeters in the Cape Peninsula</t>
+          <t>What areas are within 300 meters of runways in Schiphol airport</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Schiphol airport</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>aeroway=runway</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr">
         <is>
           <t>done</t>
@@ -1562,29 +1570,21 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
@@ -1598,11 +1598,11 @@
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z16" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="AA16" t="b">
         <v>0</v>
@@ -1610,24 +1610,28 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B17" t="n">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>What areas have an annual rainfall of more than 1000 millimeters in the Cape Peninsula</t>
+          <t>What areas are within 500 meters from religious places in Karbala in Iraq</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Karbala, Iraq</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>landuse=religious</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
           <t>done</t>
@@ -1635,29 +1639,21 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
@@ -1671,11 +1667,11 @@
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z17" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="AA17" t="b">
         <v>0</v>
@@ -1683,24 +1679,28 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B18" t="n">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>What areas have an aspect larger than 45 degree and smaller than 135 degrees in the Cape Peninsula</t>
+          <t>What areas are within 500 meters from universities in Karbala in Iraq</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Karbala, Iraq</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>amenity=university</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr">
         <is>
           <t>done</t>
@@ -1708,29 +1708,21 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Topography</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
@@ -1744,11 +1736,11 @@
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z18" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AA18" t="b">
         <v>0</v>
@@ -1756,26 +1748,26 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B19" t="n">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>What houses are larger than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
+          <t>What areas are within 60 minutes of airports in Crook, Deschutes, and Jefferson county</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Crook, Deschutes, Jefferson county</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>amenity=school, building=house</t>
+          <t xml:space="preserve"> aeroway=*</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1785,27 +1777,27 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>buffer</t>
+          <t>classification</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Data queries</t>
         </is>
       </c>
       <c r="N19" t="inlineStr"/>
@@ -1821,11 +1813,11 @@
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z19" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="AA19" t="b">
         <v>0</v>
@@ -1833,26 +1825,30 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B20" t="n">
         <v>64</v>
       </c>
-      <c r="B20" t="n">
-        <v>86</v>
-      </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>What houses are for sale and within 1km from the nearest school (from my current location) in Utrecht</t>
+          <t>What areas are within one mile of main roads in Loudoun County in US</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Utrecht</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>Loudoun County</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>amenity=school, building=house</t>
+          <t>highway=motorway</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1862,29 +1858,21 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>buffer</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
@@ -1898,11 +1886,11 @@
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z20" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="AA20" t="b">
         <v>0</v>
@@ -1910,28 +1898,28 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B21" t="n">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>What houses are for sale in flood zone in Utrecht</t>
+          <t>What areas are within two miles of urban landuse in Loudoun County in US</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Utrecht</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
+          <t>Loudoun County</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>boundary=urban, building=house</t>
-        </is>
-      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
           <t>done</t>
@@ -1939,20 +1927,24 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Data editing</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
@@ -1965,17 +1957,17 @@
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr">
         <is>
-          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
+          <t>what area는 그냥 boundary만 얘기하는 것인가? 아니면 다른 attribute도 clip하라는 것인가. 일단 clip. Urban tag를 그렇게 사용하지도 않는다</t>
         </is>
       </c>
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries,osm urban이 있긴 하지만 거의 안쓴다</t>
+          <t>data editing,data queries,buffer,overlay analysis,what area는 그냥 boundary만 얘기하는 것인가? 아니면 다른 attribute도 clip하라는 것인가. 일단 clip. urban tag를 그렇게 사용하지도 않는다</t>
         </is>
       </c>
       <c r="Z21" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="AA21" t="b">
         <v>0</v>
@@ -1983,28 +1975,24 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B22" t="n">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>What houses are greather than 30 square meters in urban areas in Utrecht</t>
+          <t>What areas do have altitude between 700 and 2000 meters in Spain</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>boundary=urban, building=house</t>
-        </is>
-      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
           <t>done</t>
@@ -2012,21 +2000,29 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Topography</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
@@ -2036,19 +2032,15 @@
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
-        </is>
-      </c>
+      <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries,osm urban이 있긴 하지만 거의 안쓴다</t>
+          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z22" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AA22" t="b">
         <v>0</v>
@@ -2056,26 +2048,26 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B23" t="n">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>What is the central feature of bank branches in Oleander</t>
+          <t>What areas do have temperature in Celsius larger than 0 degrees in Spain</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>amenity=bank</t>
+          <t>monitoring:weather=yes</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2085,21 +2077,29 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Generalization</t>
+          <t>classification</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
@@ -2108,20 +2108,16 @@
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
-        </is>
-      </c>
+      <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>data queries,generalization,geostatistics  ,https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
+          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z23" t="n">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="AA23" t="b">
         <v>0</v>
@@ -2129,28 +2125,24 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B24" t="n">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>What is the density surface of temperature measurements in Oleander city</t>
+          <t>What areas have an annual amount of snowfall more than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Oleander city</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> man_made=monitoring_station</t>
-        </is>
-      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
           <t>done</t>
@@ -2158,17 +2150,29 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
@@ -2182,11 +2186,11 @@
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z24" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="AA24" t="b">
         <v>0</v>
@@ -2194,19 +2198,19 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B25" t="n">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to green areas in Amsterdam</t>
+          <t>What areas have an annual rainfall of more than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Amsterdam</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -2219,17 +2223,29 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
@@ -2243,11 +2259,11 @@
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z25" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="AA25" t="b">
         <v>0</v>
@@ -2255,19 +2271,19 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="B26" t="n">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to the rivers in Crook, Deschutes, and Jefferson county</t>
+          <t>What areas have an aspect larger than 45 degree and smaller than 135 degrees in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Crook, Deschutes, Jefferson county</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -2280,17 +2296,29 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Topography</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
@@ -2304,11 +2332,11 @@
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z26" t="n">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="AA26" t="b">
         <v>0</v>
@@ -2316,28 +2344,28 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B27" t="n">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>What is the lung cancer mortality rate of white males for each city in the Western USA from 1970 to 1994</t>
+          <t>What houses are larger than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>the Western USA</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> from 1970 to 1994</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>amenity=school, building=house</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
           <t>done</t>
@@ -2345,7 +2373,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>network analysis</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2353,9 +2381,21 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr"/>
@@ -2369,11 +2409,11 @@
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z27" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="AA27" t="b">
         <v>0</v>
@@ -2381,24 +2421,28 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="B28" t="n">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
+          <t>What houses are for sale and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Oleander city</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>amenity=school, building=house</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
           <t>done</t>
@@ -2406,17 +2450,29 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>network analysis</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
@@ -2430,11 +2486,11 @@
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z28" t="n">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="AA28" t="b">
         <v>0</v>
@@ -2442,24 +2498,28 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="B29" t="n">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>What is the mean center of the fire calls weighted by the priority in Fort Worth</t>
+          <t>What houses are for sale and within 1km from the parks in Utrecht</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Fort Worth</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>leisure=park, building=house</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr">
         <is>
           <t>done</t>
@@ -2472,15 +2532,19 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr"/>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
@@ -2495,11 +2559,11 @@
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+          <t>data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z29" t="n">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="AA29" t="b">
         <v>0</v>
@@ -2507,28 +2571,28 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="B30" t="n">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>What is the median household income for each census block in Tarrant County in Texas</t>
+          <t>What houses are for sale in flood zone in Utrecht</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Tarrant County</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Texas</t>
-        </is>
-      </c>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>boundary=urban, building=house</t>
+        </is>
+      </c>
       <c r="H30" t="inlineStr">
         <is>
           <t>done</t>
@@ -2536,7 +2600,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2546,14 +2610,10 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>data editing</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
@@ -2564,15 +2624,19 @@
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
-      <c r="W30" t="inlineStr"/>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
+        </is>
+      </c>
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data editing,data queries</t>
+          <t>data queries,overlay analysis,data queries,osm urban이 있긴 하지만 거의 안쓴다</t>
         </is>
       </c>
       <c r="Z30" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AA30" t="b">
         <v>0</v>
@@ -2580,28 +2644,28 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="B31" t="n">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>What is the median people age for each census tract in Tarrant County in Texas</t>
+          <t>What houses are greather than 30 square meters in urban areas in Utrecht</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Tarrant County</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Texas</t>
-        </is>
-      </c>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>boundary=urban, building=house</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr">
         <is>
           <t>done</t>
@@ -2609,7 +2673,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2619,14 +2683,10 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>data editing</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr"/>
@@ -2637,15 +2697,19 @@
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="inlineStr"/>
-      <c r="W31" t="inlineStr"/>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
+        </is>
+      </c>
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data editing,data queries</t>
+          <t>data queries,overlay analysis,data queries,osm urban이 있긴 하지만 거의 안쓴다</t>
         </is>
       </c>
       <c r="Z31" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AA31" t="b">
         <v>0</v>
@@ -2653,28 +2717,24 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B32" t="n">
-        <v>149</v>
+        <v>95</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>What liquor stores are within 1000 foot of schools in El Cajon</t>
+          <t>What is the area of currently mixed use zones in Gresham</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>El Cajon</t>
+          <t>Gresham</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>shop=alcohol, amenity=school</t>
-        </is>
-      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
           <t>done</t>
@@ -2682,24 +2742,16 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Data editing</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>buffer</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
@@ -2714,11 +2766,11 @@
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries</t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="Z32" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="AA32" t="b">
         <v>0</v>
@@ -2726,30 +2778,26 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="B33" t="n">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Where are not protected region in Assam in India</t>
+          <t>Tell me the central feature of bank branches in Oleander</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+          <t>Oleander</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>landuse=conservation</t>
+          <t>amenity=bank</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2764,12 +2812,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
+          <t>Generalization</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="L33" t="inlineStr"/>
@@ -2782,16 +2830,20 @@
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
-      <c r="V33" t="inlineStr"/>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
+        </is>
+      </c>
       <c r="W33" t="inlineStr"/>
       <c r="X33" t="inlineStr"/>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data queries,generalization,geostatistics  ,https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
         </is>
       </c>
       <c r="Z33" t="n">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AA33" t="b">
         <v>0</v>
@@ -2799,26 +2851,26 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="B34" t="n">
-        <v>156</v>
+        <v>105</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Where are the commercial areas in Amsterdam</t>
+          <t>What is the central feature of bank branches in Oleander</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Amsterdam</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>landuse=commercial</t>
+          <t>amenity=bank</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2833,12 +2885,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
+          <t>Generalization</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
@@ -2851,16 +2903,20 @@
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
-      <c r="V34" t="inlineStr"/>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
+        </is>
+      </c>
       <c r="W34" t="inlineStr"/>
       <c r="X34" t="inlineStr"/>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data queries,generalization,geostatistics  ,https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
         </is>
       </c>
       <c r="Z34" t="n">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AA34" t="b">
         <v>0</v>
@@ -2868,26 +2924,26 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="B35" t="n">
-        <v>164</v>
+        <v>111</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Where are the rocky areas in Spain</t>
+          <t>What is the density surface of rainfall measurements in the Netherlands</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>the Netherlands</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>nature : bare_rock</t>
+          <t xml:space="preserve"> man_made=monitoring_station</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2902,14 +2958,10 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
@@ -2925,11 +2977,11 @@
       <c r="X35" t="inlineStr"/>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z35" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AA35" t="b">
         <v>0</v>
@@ -2937,26 +2989,26 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="B36" t="n">
-        <v>167</v>
+        <v>112</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Which houses are for sale in Utrecht</t>
+          <t>What is the density surface of temperature measurements in Oleander city</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Oleander city</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>building=house</t>
+          <t xml:space="preserve"> man_made=monitoring_station</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2966,12 +3018,12 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
@@ -2990,11 +3042,11 @@
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z36" t="n">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="AA36" t="b">
         <v>0</v>
@@ -3002,28 +3054,24 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="B37" t="n">
-        <v>170</v>
+        <v>115</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Which houses have construction year between 1990 and 2000 in Utrecht</t>
+          <t>What is the Euclidean distance to green areas in Amsterdam</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Amsterdam</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>year_of_construction=*</t>
-        </is>
-      </c>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
           <t>done</t>
@@ -3034,7 +3082,11 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
@@ -3051,11 +3103,11 @@
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z37" t="n">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="AA37" t="b">
         <v>0</v>
@@ -3063,28 +3115,24 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>133</v>
+        <v>94</v>
       </c>
       <c r="B38" t="n">
-        <v>177</v>
+        <v>120</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Which schools are not within 3 minutes of driving time from a fire station in Fort Worth</t>
+          <t>What is the Euclidean distance to the rivers in Crook, Deschutes, and Jefferson county</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Fort Worth</t>
+          <t>Crook, Deschutes, Jefferson county</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>amenity=fire_station, amenity=school</t>
-        </is>
-      </c>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
           <t>done</t>
@@ -3097,29 +3145,13 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Network analysis</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
@@ -3132,11 +3164,11 @@
       <c r="X38" t="inlineStr"/>
       <c r="Y38" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z38" t="n">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="AA38" t="b">
         <v>0</v>
@@ -3144,28 +3176,28 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B39" t="n">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Which vacant lots are within 1 mile of a freeway in Hillsboro</t>
+          <t>What is the lung cancer mortality rate of white males for each city in the Western USA from 1970 to 1994</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Hillsboro</t>
+          <t>the Western USA</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>abandoned:*=*, highway=motorway</t>
-        </is>
-      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> from 1970 to 1994</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
           <t>done</t>
@@ -3173,24 +3205,16 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>buffer</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
@@ -3205,11 +3229,11 @@
       <c r="X39" t="inlineStr"/>
       <c r="Y39" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries</t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="Z39" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="AA39" t="b">
         <v>0</v>
@@ -3217,28 +3241,24 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="B40" t="n">
-        <v>183</v>
+        <v>129</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Which wind farm proposals are nearest to the high way in Scotland</t>
+          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Scotland</t>
+          <t>Oleander city</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>highway=*</t>
-        </is>
-      </c>
+      <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
           <t>done</t>
@@ -3251,14 +3271,10 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>network analysis</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
@@ -3274,11 +3290,11 @@
       <c r="X40" t="inlineStr"/>
       <c r="Y40" t="inlineStr">
         <is>
-          <t>data queries,network analysis,data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z40" t="n">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="AA40" t="b">
         <v>0</v>
@@ -3286,28 +3302,24 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="B41" t="n">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Which wind farm proposals are nearest to the roads in Scotland</t>
+          <t>What is the weighted coordinate average of library patrons for each district in Oleander</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Scotland</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>highway=*</t>
-        </is>
-      </c>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
           <t>done</t>
@@ -3320,12 +3332,12 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="L41" t="inlineStr"/>
@@ -3343,13 +3355,1352 @@
       <c r="X41" t="inlineStr"/>
       <c r="Y41" t="inlineStr">
         <is>
+          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+        </is>
+      </c>
+      <c r="Z41" t="n">
+        <v>44</v>
+      </c>
+      <c r="AA41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B42" t="n">
+        <v>134</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>What is the mean center of the fire calls weighted by the priority in Fort Worth</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr"/>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+        </is>
+      </c>
+      <c r="Z42" t="n">
+        <v>44</v>
+      </c>
+      <c r="AA42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B43" t="n">
+        <v>136</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Tell me the median household income for each census block in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Texas</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr"/>
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t>data editing,overlay analysis,data editing,data queries</t>
+        </is>
+      </c>
+      <c r="Z43" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B44" t="n">
+        <v>139</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>What is the median household income for each census block in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Texas</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr"/>
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t>data editing,overlay analysis,data editing,data queries</t>
+        </is>
+      </c>
+      <c r="Z44" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B45" t="n">
+        <v>141</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>What is the median people age for each census tract in Tarrant County in Texas</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Texas</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
+      <c r="X45" t="inlineStr"/>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>data editing,overlay analysis,data editing,data queries</t>
+        </is>
+      </c>
+      <c r="Z45" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B46" t="n">
+        <v>146</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>What is the population density in California</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>population</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr"/>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
+      <c r="X46" t="inlineStr"/>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data editing,data queries</t>
+        </is>
+      </c>
+      <c r="Z46" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B47" t="n">
+        <v>149</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>What liquor stores are within 1000 foot of schools in El Cajon</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>El Cajon</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>shop=alcohol, amenity=school</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr"/>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>data queries,buffer,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z47" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B48" t="n">
+        <v>153</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Where are not protected region in Assam in India</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Assam</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>landuse=conservation</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="Z48" t="n">
+        <v>47</v>
+      </c>
+      <c r="AA48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B49" t="n">
+        <v>156</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Where are the commercial areas in Amsterdam</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Amsterdam</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>landuse=commercial</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="Z49" t="n">
+        <v>47</v>
+      </c>
+      <c r="AA49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B50" t="n">
+        <v>164</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Where are the rocky areas in Spain</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>nature : bare_rock</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="Z50" t="n">
+        <v>47</v>
+      </c>
+      <c r="AA50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B51" t="n">
+        <v>167</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Which houses are for sale in Utrecht</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>building=house</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr"/>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>data editing,data queries</t>
+        </is>
+      </c>
+      <c r="Z51" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B52" t="n">
+        <v>170</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Which houses have construction year between 1990 and 2000 in Utrecht</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>year_of_construction=*</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>data queries</t>
+        </is>
+      </c>
+      <c r="Z52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B53" t="n">
+        <v>171</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Which land use contains meteorological stations in Netherlands</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> man_made=monitoring_station</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>data queries,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B54" t="n">
+        <v>173</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Which park is biggest in Utrecht</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>leisure=park</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="Z54" t="n">
+        <v>47</v>
+      </c>
+      <c r="AA54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B55" t="n">
+        <v>174</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Which schools are not accessible within 3 minutes by a car from a fire station in Fort Worth</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>amenity=fire_station, amenity=school</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>data queries</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z55" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B56" t="n">
+        <v>177</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Which schools are not within 3 minutes of driving time from a fire station in Fort Worth</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>amenity=fire_station, amenity=school</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>data queries</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z56" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B57" t="n">
+        <v>179</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Which vacant lots are within 1 mile of a freeway in Hillsboro</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Hillsboro</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>abandoned:*=*, highway=motorway</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>data queries,buffer,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z57" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B58" t="n">
+        <v>180</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Which visitor facilities are in the Happy Valley</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>the Happy Valley</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>information=visitor_centre</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr"/>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>data queries</t>
+        </is>
+      </c>
+      <c r="Z58" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B59" t="n">
+        <v>183</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Which wind farm proposals are nearest to the high way in Scotland</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>highway=*</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>network analysis</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr"/>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr"/>
+      <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr"/>
+      <c r="Y59" t="inlineStr">
+        <is>
           <t>data queries,network analysis,data queries</t>
         </is>
       </c>
-      <c r="Z41" t="n">
+      <c r="Z59" t="n">
         <v>4</v>
       </c>
-      <c r="AA41" t="b">
+      <c r="AA59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B60" t="n">
+        <v>185</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Which wind farm proposals are nearest to the roads in Scotland</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>highway=*</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>network analysis</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="inlineStr"/>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="inlineStr"/>
+      <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr"/>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>data queries,network analysis,data queries</t>
+        </is>
+      </c>
+      <c r="Z60" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA60" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Paraphrase and drop column "unamed"
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/stratified_test.xlsx
+++ b/textToOps/data/processed/stratified_test.xlsx
@@ -567,19 +567,19 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What are the areas within a four-minute drive of each fire station at 2 a.m. on Tuesday in Utrecht</t>
+          <t>What areas are more than 5000 meters from the roads in Spain</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -597,29 +597,17 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
@@ -632,11 +620,11 @@
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z2" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="AA2" t="b">
         <v>0</v>
@@ -644,19 +632,19 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>What are the four fire stations within 3 minutes of travel time from a fire in San Francisco</t>
+          <t>Tell me not flood plain area in Houston</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -674,29 +662,13 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Network analysis</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
@@ -709,11 +681,11 @@
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+          <t>data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z3" t="n">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="AA3" t="b">
         <v>0</v>
@@ -721,19 +693,19 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>What are the land use inside the flood zones in Oleander</t>
+          <t>What areas are not conatined as green belt areas in Houston</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -754,11 +726,7 @@
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
@@ -774,11 +742,11 @@
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries</t>
+          <t>data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z4" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="AA4" t="b">
         <v>0</v>
@@ -786,26 +754,26 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B5" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>What are the vegetation areas larger than 6000 square meters in the Cape Peninsula</t>
+          <t>What areas are not wetlands in Houston</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">nature : glacier, landuse =forest, wetland=mangrove </t>
+          <t>natural=wetland</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -818,16 +786,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Geometry measurement</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
@@ -839,19 +799,15 @@
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>Vegetation 애매함. OSM만으로 불가.</t>
-        </is>
-      </c>
+      <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="Z5" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AA5" t="b">
         <v>0</v>
@@ -859,30 +815,26 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B6" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>What area are within 50 km from family physician services in Saskatchewan in Canada</t>
+          <t>What areas are outside 150 meters from schools in Houston</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Saskatchewan</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>amenity=doctor</t>
+          <t>amenity=school</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -932,26 +884,30 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B7" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>What areas are inside 1000 foot of schools in El Cajon</t>
+          <t>What areas are outside 5 km of water bodies in Assam in India</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>El Cajon</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>Assam</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>amenity=school, amenity=kindergarten</t>
+          <t>landuse=aquaculture, basin, salt_pond</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1001,24 +957,28 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B8" t="n">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>What areas are green belt areas in Houston</t>
+          <t>What areas are outside 5000 meters of the roads in Spain</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>highway=*</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
           <t>done</t>
@@ -1031,10 +991,14 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
@@ -1050,11 +1014,11 @@
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AA8" t="b">
         <v>0</v>
@@ -1062,14 +1026,14 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B9" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>What areas are not conatined as green belt areas in Houston</t>
+          <t>What areas are outside 60 meters from residence in Houston</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1079,7 +1043,11 @@
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>residential=*</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>done</t>
@@ -1092,10 +1060,14 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
@@ -1111,11 +1083,11 @@
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z9" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AA9" t="b">
         <v>0</v>
@@ -1123,26 +1095,26 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>What areas are not park in Houston</t>
+          <t>What areas are within 100 meters of cameras in Salford</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Salford</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>leisure=park</t>
+          <t>man_made=surveillance, highway=speed_camera</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1155,8 +1127,16 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
@@ -1168,15 +1148,19 @@
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>정확히 카메라가 무엇을 뜻하는가</t>
+        </is>
+      </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA10" t="b">
         <v>0</v>
@@ -1184,26 +1168,26 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B11" t="n">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>What areas are not wetlands in Houston</t>
+          <t>What areas are within 1000 meters of the arcades in Oleander</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>natural=wetland</t>
+          <t>leisure=amusement_arcade</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1216,8 +1200,16 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Buffer</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
@@ -1233,11 +1225,11 @@
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z11" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA11" t="b">
         <v>0</v>
@@ -1245,26 +1237,26 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B12" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>What areas are outside 250 meters of human settlement in the Cape Peninsula</t>
+          <t>What areas are within 1000 meters of the major transport routes in Amsterdam</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Amsterdam</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>residential=*</t>
+          <t>highway=motorway</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1298,7 +1290,11 @@
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>major가 무엇인지</t>
+        </is>
+      </c>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr">
         <is>
@@ -1314,28 +1310,24 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B13" t="n">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>What areas are outside 3000 meters of the rivers in Spain</t>
+          <t>What areas are outside 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>waterway=river</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>done</t>
@@ -1348,18 +1340,34 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
@@ -1367,15 +1375,19 @@
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>어디로 부터 가장 가까운 소방서</t>
+        </is>
+      </c>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z13" t="n">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="AA13" t="b">
         <v>0</v>
@@ -1383,28 +1395,24 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B14" t="n">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>What areas are within 10 miles of current transmission lines with a voltage greater than 400 in Colorado</t>
+          <t>What areas are within 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>power=line</t>
-        </is>
-      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>done</t>
@@ -1417,18 +1425,34 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
@@ -1436,15 +1460,19 @@
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>어디로 부터 가장 가까운 소방서</t>
+        </is>
+      </c>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z14" t="n">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="AA14" t="b">
         <v>0</v>
@@ -1452,30 +1480,26 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B15" t="n">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>What areas are within 1000 meters of roads in Assam in India</t>
+          <t>What areas are within 500 meters from religious places in Karbala in Iraq</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+          <t>Karbala, Iraq</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>highway=*</t>
+          <t>landuse=religious</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1509,11 +1533,7 @@
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>matter of scale. 도로는 line인가</t>
-        </is>
-      </c>
+      <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr">
         <is>
@@ -1529,28 +1549,28 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B16" t="n">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>What areas are within 1000 meters of the schools in Oleander</t>
+          <t>What areas are accessible within two miles of urban landuse in Loudoun County in US</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Oleander</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>Loudoun County</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>amenity=school</t>
-        </is>
-      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>done</t>
@@ -1558,20 +1578,24 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Data editing</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
           <t>Buffer</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
@@ -1582,15 +1606,19 @@
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>what area는 그냥 boundary만 얘기하는 것인가? 아니면 다른 attribute도 clip하라는 것인가. 일단 clip. Urban tag를 그렇게 사용하지도 않는다</t>
+        </is>
+      </c>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data editing,data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z16" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AA16" t="b">
         <v>0</v>
@@ -1598,19 +1626,19 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B17" t="n">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>What areas are accessible within 3 minutes of by car from the nearest fire station (from my current location) in Oleander</t>
+          <t>What areas have an monthly rainfall of more than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -1623,12 +1651,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>classification</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1638,24 +1666,16 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Data model conversion</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
@@ -1663,19 +1683,15 @@
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>어디로 부터 가장 가까운 소방서</t>
-        </is>
-      </c>
+      <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z17" t="n">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AA17" t="b">
         <v>0</v>
@@ -1683,19 +1699,19 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B18" t="n">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>What areas are within 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
+          <t>What areas have an annual amount of snowfall more than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1708,12 +1724,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>classification</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1723,24 +1739,16 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Data model conversion</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
@@ -1748,19 +1756,15 @@
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>어디로 부터 가장 가까운 소방서</t>
-        </is>
-      </c>
+      <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z18" t="n">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AA18" t="b">
         <v>0</v>
@@ -1768,28 +1772,24 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="B19" t="n">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>What areas are within 300 meters of runways in Schiphol airport</t>
+          <t>What areas have slope larger than 15 percent and smaller than 60 percent in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Schiphol airport</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>aeroway=runway</t>
-        </is>
-      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
           <t>done</t>
@@ -1797,21 +1797,29 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Topography</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>classification</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
@@ -1825,11 +1833,11 @@
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z19" t="n">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="AA19" t="b">
         <v>0</v>
@@ -1837,26 +1845,26 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="B20" t="n">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>What areas are within 60 minutes of airports in Crook, Deschutes, and Jefferson county</t>
+          <t>What houses are less than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Crook, Deschutes, Jefferson county</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> aeroway=*</t>
+          <t>amenity=school, building=house</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1866,27 +1874,27 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>network analysis</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>buffer</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="N20" t="inlineStr"/>
@@ -1902,11 +1910,11 @@
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z20" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AA20" t="b">
         <v>0</v>
@@ -1914,26 +1922,26 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B21" t="n">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>What areas are within a quarter mile of light rail stop in Gresham</t>
+          <t>What houses are for sale and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Gresham</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>railway=tram_stop, light_rail</t>
+          <t>amenity=school, building=house</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1943,21 +1951,29 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>network analysis</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
@@ -1971,11 +1987,11 @@
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z21" t="n">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="AA21" t="b">
         <v>0</v>
@@ -1983,28 +1999,28 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B22" t="n">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>What areas are within two miles of urban landuse in Loudoun County in US</t>
+          <t>What houses are for sale outside flood zone in Utrecht</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Loudoun County</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>boundary=urban, building=house</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr">
         <is>
           <t>done</t>
@@ -2012,24 +2028,20 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Buffer</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
@@ -2042,17 +2054,17 @@
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="inlineStr">
         <is>
-          <t>what area는 그냥 boundary만 얘기하는 것인가? 아니면 다른 attribute도 clip하라는 것인가. 일단 clip. Urban tag를 그렇게 사용하지도 않는다</t>
+          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
         </is>
       </c>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>data editing,data queries,buffer,overlay analysis</t>
+          <t>data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z22" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="AA22" t="b">
         <v>0</v>
@@ -2060,24 +2072,28 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B23" t="n">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>What areas have an annual amount of snowfall more than 1000 millimeters in the Cape Peninsula</t>
+          <t>What houses are for sale in flood zone in Utrecht</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>boundary=urban, building=house</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr">
         <is>
           <t>done</t>
@@ -2085,12 +2101,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2098,16 +2114,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
@@ -2117,15 +2125,19 @@
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr"/>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
+        </is>
+      </c>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z23" t="n">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="AA23" t="b">
         <v>0</v>
@@ -2133,24 +2145,28 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B24" t="n">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>What areas have an annual rainfall of more than 1000 millimeters in the Cape Peninsula</t>
+          <t>What houses are larger than 30 square meters in urban areas in Utrecht</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>boundary=urban, building=house</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
           <t>done</t>
@@ -2158,12 +2174,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2171,16 +2187,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
@@ -2190,15 +2198,19 @@
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
-      <c r="W24" t="inlineStr"/>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
+        </is>
+      </c>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z24" t="n">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="AA24" t="b">
         <v>0</v>
@@ -2206,24 +2218,28 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B25" t="n">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>What areas have an aspect larger than 45 degree and smaller than 135 degrees in the Cape Peninsula</t>
+          <t>What is weighted average coordinates of bank branches in Oleander</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>amenity=bank</t>
+        </is>
+      </c>
       <c r="H25" t="inlineStr">
         <is>
           <t>done</t>
@@ -2231,29 +2247,21 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Topography</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Generalization</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
@@ -2262,16 +2270,20 @@
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
+        </is>
+      </c>
       <c r="W25" t="inlineStr"/>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
+          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
         </is>
       </c>
       <c r="Z25" t="n">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AA25" t="b">
         <v>0</v>
@@ -2279,26 +2291,26 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="B26" t="n">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>What houses are larger than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
+          <t>What is the central feature of bank branches in Oleander</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>amenity=school, building=house</t>
+          <t>amenity=bank</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2308,29 +2320,21 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Generalization</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>buffer</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
@@ -2339,16 +2343,20 @@
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr"/>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
+        </is>
+      </c>
       <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
+          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
         </is>
       </c>
       <c r="Z26" t="n">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="AA26" t="b">
         <v>0</v>
@@ -2356,28 +2364,28 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B27" t="n">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>What houses are for sale and within 1km from the nearest school (from my current location) in Utrecht</t>
+          <t>What is the cervix cancer mortality rate of white females for each city in the Western USA from 1970 to 1994</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t xml:space="preserve">the Western USA </t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>amenity=school, building=house</t>
-        </is>
-      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>from 1970 to 1994</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
           <t>done</t>
@@ -2385,7 +2393,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Data editing</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2393,21 +2401,9 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>buffer</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr"/>
@@ -2421,11 +2417,11 @@
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="Z27" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="AA27" t="b">
         <v>0</v>
@@ -2433,28 +2429,24 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="B28" t="n">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>What houses are for sale outside flood zone in Utrecht</t>
+          <t>What is the Euclidean distance to green areas in Amsterdam</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Amsterdam</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>boundary=urban, building=house</t>
-        </is>
-      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
           <t>done</t>
@@ -2467,14 +2459,10 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
@@ -2486,19 +2474,15 @@
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
-        </is>
-      </c>
+      <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z28" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AA28" t="b">
         <v>0</v>
@@ -2506,26 +2490,26 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B29" t="n">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>What houses are for sale in urban areas in Utrecht</t>
+          <t>What is the Euclidean distance to hospitals in Oleander</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>boundary=urban, building=house</t>
+          <t>amenity=hospital</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2540,14 +2524,10 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
@@ -2559,19 +2539,15 @@
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
       <c r="V29" t="inlineStr"/>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
-        </is>
-      </c>
+      <c r="W29" t="inlineStr"/>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z29" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AA29" t="b">
         <v>0</v>
@@ -2579,24 +2555,28 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B30" t="n">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>What is the area of currently mixed use zones in Gresham</t>
+          <t>What is the Euclidean distance to schools in Utrecht</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Gresham</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>amenity=school</t>
+        </is>
+      </c>
       <c r="H30" t="inlineStr">
         <is>
           <t>done</t>
@@ -2604,12 +2584,12 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
@@ -2628,11 +2608,11 @@
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z30" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AA30" t="b">
         <v>0</v>
@@ -2640,28 +2620,24 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B31" t="n">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Tell me the central feature of bank branches in Oleander</t>
+          <t>What is the interpolated surface of ozone concentration in California</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>California</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>amenity=bank</t>
-        </is>
-      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
           <t>done</t>
@@ -2669,12 +2645,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Data editing</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Generalization</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2692,20 +2668,16 @@
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
-      <c r="V31" t="inlineStr">
-        <is>
-          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
-        </is>
-      </c>
+      <c r="V31" t="inlineStr"/>
       <c r="W31" t="inlineStr"/>
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
+          <t xml:space="preserve">data editing,data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z31" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AA31" t="b">
         <v>0</v>
@@ -2713,26 +2685,26 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="B32" t="n">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>What is the central feature of bank branches in Oleander</t>
+          <t>What is the land use in Netherlands</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>amenity=bank</t>
+          <t>landuse=*</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2745,16 +2717,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Generalization</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
@@ -2765,20 +2729,16 @@
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
-      <c r="V32" t="inlineStr">
-        <is>
-          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
-        </is>
-      </c>
+      <c r="V32" t="inlineStr"/>
       <c r="W32" t="inlineStr"/>
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="Z32" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AA32" t="b">
         <v>0</v>
@@ -2786,27 +2746,23 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="B33" t="n">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>What is the cervix cancer mortality rate of white females for each city in the Western USA from 1970 to 1994</t>
+          <t>What is the literacy rate for each country in Africa</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">the Western USA </t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>from 1970 to 1994</t>
-        </is>
-      </c>
+      <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
@@ -2815,7 +2771,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Data editing</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2851,14 +2807,14 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="B34" t="n">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>What is the density surface of temperature measurements in Oleander city</t>
+          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2868,11 +2824,7 @@
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> man_made=monitoring_station</t>
-        </is>
-      </c>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
           <t>done</t>
@@ -2916,23 +2868,27 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B35" t="n">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to green areas in Amsterdam</t>
+          <t>What is the mean center of the fire calls for each alarm territory in Fort Worth in 2017</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Amsterdam</t>
+          <t>Fort Worth</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
@@ -2946,10 +2902,14 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
           <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
-      <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
@@ -2965,11 +2925,11 @@
       <c r="X35" t="inlineStr"/>
       <c r="Y35" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
         </is>
       </c>
       <c r="Z35" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="AA35" t="b">
         <v>0</v>
@@ -2977,22 +2937,26 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="B36" t="n">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to the rivers in Crook, Deschutes, and Jefferson county</t>
+          <t>What is the median population for each census block in Tarrant County in Texas</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Crook, Deschutes, Jefferson county</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>Tarrant County</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Texas</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
@@ -3002,16 +2966,24 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
@@ -3026,11 +2998,11 @@
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>data editing,overlay analysis,data editing,data queries</t>
         </is>
       </c>
       <c r="Z36" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="AA36" t="b">
         <v>0</v>
@@ -3038,19 +3010,19 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="B37" t="n">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>What is the interpolation surface of NO2 concentration in Vancouver</t>
+          <t>What is the number of arson cases in Fort Worth on February 2004</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Fort Worth on February 2004</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -3063,7 +3035,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Data editing</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -3071,11 +3043,7 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
+      <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
@@ -3091,11 +3059,11 @@
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr">
         <is>
-          <t xml:space="preserve">data editing,data queries,geostatistics  </t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="Z37" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="AA37" t="b">
         <v>0</v>
@@ -3103,19 +3071,19 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B38" t="n">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
+          <t>What is the number of buildings within 3 minutes of driving time from fire stations in Oleander</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Oleander city</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -3133,13 +3101,29 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
@@ -3152,11 +3136,11 @@
       <c r="X38" t="inlineStr"/>
       <c r="Y38" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z38" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="AA38" t="b">
         <v>0</v>
@@ -3164,19 +3148,19 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B39" t="n">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>What is the mean center of the fire calls weighted by the priority in Fort Worth</t>
+          <t>What is the number of high school students for each senior high school district in Oleander</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Fort Worth</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -3189,20 +3173,24 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr"/>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
@@ -3217,11 +3205,11 @@
       <c r="X39" t="inlineStr"/>
       <c r="Y39" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+          <t>data editing,data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z39" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="AA39" t="b">
         <v>0</v>
@@ -3229,14 +3217,14 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B40" t="n">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>What is the median household income for each census block in Tarrant County in Texas</t>
+          <t>What is the number of Hispanics for each census block in Tarrant County in Texas</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3246,7 +3234,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Texas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
@@ -3263,12 +3251,12 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>data editing</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3290,11 +3278,11 @@
       <c r="X40" t="inlineStr"/>
       <c r="Y40" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data editing,data queries</t>
+          <t>data editing,data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z40" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA40" t="b">
         <v>0</v>
@@ -3302,27 +3290,27 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="B41" t="n">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>What is the median people age for each census tract in Tarrant County in Texas</t>
+          <t xml:space="preserve">What is the number of injured pedestrians for each census tract in Georgia from 2000 to 2007 </t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Tarrant County</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Texas</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr"/>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> from 2000 to 2007 </t>
+        </is>
+      </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
@@ -3375,26 +3363,22 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B42" t="n">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>What is the number of Hispanics for each census block in Tarrant County in Texas</t>
+          <t>What is the number of luxury hotels in Happy Valley ski resort</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Tarrant County</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Texas</t>
-        </is>
-      </c>
+          <t>Happy Valley ski resort</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
@@ -3404,24 +3388,12 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>data editing</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr"/>
@@ -3436,11 +3408,11 @@
       <c r="X42" t="inlineStr"/>
       <c r="Y42" t="inlineStr">
         <is>
-          <t>data editing,data queries,overlay analysis,data queries</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="Z42" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="AA42" t="b">
         <v>0</v>
@@ -3448,26 +3420,22 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B43" t="n">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>What is the number of inhabitants for each village in Banten province in Indonesia</t>
+          <t>What is the point density of fire calls in Oleander</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Banten province</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Indonesia</t>
-        </is>
-      </c>
+          <t>Oleander</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -3492,7 +3460,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="M43" t="inlineStr"/>
@@ -3509,11 +3477,11 @@
       <c r="X43" t="inlineStr"/>
       <c r="Y43" t="inlineStr">
         <is>
-          <t>data editing,data queries,overlay analysis,data queries</t>
+          <t xml:space="preserve">data editing,data queries,overlay analysis,geostatistics  </t>
         </is>
       </c>
       <c r="Z43" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="AA43" t="b">
         <v>0</v>
@@ -3521,28 +3489,28 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B44" t="n">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>What is the point density of cycling destinations in the Metro Vancouver region in Canada</t>
+          <t>What is the total area of agriculture in Netherlands</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>the Metro Vancouver region</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>agriculture=*, landuse=argiculture</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr">
         <is>
           <t>done</t>
@@ -3550,22 +3518,22 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
           <t>data editing</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="M44" t="inlineStr"/>
@@ -3582,11 +3550,11 @@
       <c r="X44" t="inlineStr"/>
       <c r="Y44" t="inlineStr">
         <is>
-          <t xml:space="preserve">data editing,data queries,overlay analysis,geostatistics  </t>
+          <t>data queries,geometry measurement,data editing,data queries</t>
         </is>
       </c>
       <c r="Z44" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA44" t="b">
         <v>0</v>
@@ -3594,28 +3562,24 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B45" t="n">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>What is the population density in California</t>
+          <t>What is the total population within a four-minute travel time from fire stations in Poway</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Poway</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>population</t>
-        </is>
-      </c>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
           <t>done</t>
@@ -3628,12 +3592,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>classification</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3641,8 +3605,16 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
@@ -3655,11 +3627,11 @@
       <c r="X45" t="inlineStr"/>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data editing,data queries</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z45" t="n">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="AA45" t="b">
         <v>0</v>
@@ -3667,28 +3639,28 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B46" t="n">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>What is the tornado path in Oleander in April 2011</t>
+          <t>What liquor stores are within 1000 foot of parks in El Cajon</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>El Cajon</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>April 2011</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>shop=alcohol, leisure=park</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr">
         <is>
           <t>done</t>
@@ -3696,16 +3668,24 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
@@ -3720,11 +3700,11 @@
       <c r="X46" t="inlineStr"/>
       <c r="Y46" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t>data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z46" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="AA46" t="b">
         <v>0</v>
@@ -3805,26 +3785,30 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B48" t="n">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Where are forestry lands in Happy Valley ski resort</t>
+          <t>Where are not protected region in Assam in India</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Happy Valley ski resort</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
+          <t>Assam</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Tag:landuse=forestry</t>
+          <t>landuse=conservation</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3837,8 +3821,16 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr"/>
-      <c r="K48" t="inlineStr"/>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr"/>
@@ -3854,11 +3846,11 @@
       <c r="X48" t="inlineStr"/>
       <c r="Y48" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t>data queries,geometry measurement,data queries</t>
         </is>
       </c>
       <c r="Z48" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AA48" t="b">
         <v>0</v>
@@ -3866,26 +3858,26 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B49" t="n">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Where are not conservation areas in UK</t>
+          <t>Where are the commercial areas in Amsterdam</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Amsterdam</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>landuse=conservation</t>
+          <t>landuse=commercial</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3935,32 +3927,24 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B50" t="n">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Where are not protected region in Assam in India</t>
+          <t>Where are the five star hotels in the Happy Valley ski resort</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+          <t>the Happy Valley ski resort</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>landuse=conservation</t>
-        </is>
-      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
           <t>done</t>
@@ -4008,26 +3992,26 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B51" t="n">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Where are the industrial areas in Utrecht</t>
+          <t>Which houses are within 2 minutes driving time from fire stations  (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>landuse=industrial</t>
+          <t>amenity=fire_station</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4042,16 +4026,24 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
@@ -4065,11 +4057,11 @@
       <c r="X51" t="inlineStr"/>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z51" t="n">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="AA51" t="b">
         <v>0</v>
@@ -4077,26 +4069,26 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B52" t="n">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Which schools are not reachable within 3 minutes of driving time from a fire station in Fort Worth</t>
+          <t>Which park is biggest in Utrecht</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Fort Worth</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>amenity=fire_station, amenity=school</t>
+          <t>leisure=park</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4111,29 +4103,17 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Geometry measurement</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
@@ -4146,11 +4126,11 @@
       <c r="X52" t="inlineStr"/>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+          <t>data queries,geometry measurement,data queries</t>
         </is>
       </c>
       <c r="Z52" t="n">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="AA52" t="b">
         <v>0</v>
@@ -4158,26 +4138,26 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B53" t="n">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Which vacant lots are within 1 mile of a freeway in Hillsboro</t>
+          <t>Which schools are not accessible within 3 minutes by a car from a fire station in Fort Worth</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Hillsboro</t>
+          <t>Fort Worth</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>abandoned:*=*, highway=motorway</t>
+          <t>amenity=fire_station, amenity=school</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4192,21 +4172,29 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>data queries</t>
+        </is>
+      </c>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
@@ -4219,11 +4207,11 @@
       <c r="X53" t="inlineStr"/>
       <c r="Y53" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z53" t="n">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="AA53" t="b">
         <v>0</v>
@@ -4231,14 +4219,14 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B54" t="n">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Which wind farm proposals are nearest to the high way in Scotland</t>
+          <t>Which proposed wind farm are nearest to the high way in Scotland</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4300,14 +4288,14 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B55" t="n">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Which wind farm proposals are nearest to the roads in Scotland</t>
+          <t>Which wind farm proposals are nearest to the high way in Scotland</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">

</xml_diff>

<commit_message>
paraphrase by change params
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/stratified_test.xlsx
+++ b/textToOps/data/processed/stratified_test.xlsx
@@ -567,24 +567,28 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What areas are more than 5000 meters from the roads in Spain</t>
+          <t>What are the four fire stations with shortest network-based paths to 1202 Twin Peaks Blvd in San Francisco</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>highway=*, name=Twin Peaks Boulevard, amenity=fire_station</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>done</t>
@@ -597,12 +601,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
@@ -620,11 +624,11 @@
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,network analysis,data queries</t>
         </is>
       </c>
       <c r="Z2" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AA2" t="b">
         <v>0</v>
@@ -632,19 +636,19 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tell me not flood plain area in Houston</t>
+          <t>What are the four fire stations within 3 minutes of travel time from a fire in San Francisco</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -662,13 +666,29 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
@@ -681,11 +701,11 @@
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z3" t="n">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="AA3" t="b">
         <v>0</v>
@@ -693,14 +713,14 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>What areas are not conatined as green belt areas in Houston</t>
+          <t>What areas are not flood plain in Houston</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -754,14 +774,14 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>What areas are not wetlands in Houston</t>
+          <t>Tell me not flood plain area in Houston</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -771,11 +791,7 @@
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>natural=wetland</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>done</t>
@@ -786,7 +802,11 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
@@ -803,11 +823,11 @@
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t>data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA5" t="b">
         <v>0</v>
@@ -815,14 +835,14 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>What areas are outside 150 meters from schools in Houston</t>
+          <t>What areas are outside 155 meters from nature reserve districts in Houston</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -834,7 +854,7 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>amenity=school</t>
+          <t>leisure=nature_reserve</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -884,30 +904,26 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>What areas are outside 5 km of water bodies in Assam in India</t>
+          <t>What areas are outside 3000 meters of the rivers in Spain</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>landuse=aquaculture, basin, salt_pond</t>
+          <t>waterway=river</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1026,26 +1042,26 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B9" t="n">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>What areas are outside 60 meters from residence in Houston</t>
+          <t>What areas are within 1000 meters of the major transport routes in Amsterdam</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Amsterdam</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>residential=*</t>
+          <t>highway=motorway</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1079,7 +1095,11 @@
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>major가 무엇인지</t>
+        </is>
+      </c>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr">
         <is>
@@ -1095,28 +1115,24 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B10" t="n">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>What areas are within 100 meters of cameras in Salford</t>
+          <t>What areas are reachable within 3 minutes of by car from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Salford</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>man_made=surveillance, highway=speed_camera</t>
-        </is>
-      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>done</t>
@@ -1129,18 +1145,34 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
@@ -1150,17 +1182,17 @@
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr">
         <is>
-          <t>정확히 카메라가 무엇을 뜻하는가</t>
+          <t>어디로 부터 가장 가까운 소방서</t>
         </is>
       </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z10" t="n">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="AA10" t="b">
         <v>0</v>
@@ -1168,14 +1200,14 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B11" t="n">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>What areas are within 1000 meters of the arcades in Oleander</t>
+          <t>What areas are outside 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1185,11 +1217,7 @@
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>leisure=amusement_arcade</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>done</t>
@@ -1202,18 +1230,34 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Buffer</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Network analysis</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
@@ -1221,15 +1265,19 @@
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>어디로 부터 가장 가까운 소방서</t>
+        </is>
+      </c>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis</t>
+          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z11" t="n">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="AA11" t="b">
         <v>0</v>
@@ -1237,26 +1285,26 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B12" t="n">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>What areas are within 1000 meters of the major transport routes in Amsterdam</t>
+          <t>What areas are within 500 meters from religious places in Karbala in Iraq</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Amsterdam</t>
+          <t>Karbala, Iraq</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>highway=motorway</t>
+          <t>landuse=religious</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1290,11 +1338,7 @@
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>major가 무엇인지</t>
-        </is>
-      </c>
+      <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr">
         <is>
@@ -1310,24 +1354,28 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B13" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>What areas are outside 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
+          <t>What areas are within 500 meters from universities in Karbala in Iraq</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Karbala, Iraq</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>amenity=university</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
           <t>done</t>
@@ -1340,34 +1388,18 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>Network analysis</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
@@ -1375,19 +1407,15 @@
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>어디로 부터 가장 가까운 소방서</t>
-        </is>
-      </c>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z13" t="n">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="AA13" t="b">
         <v>0</v>
@@ -1395,24 +1423,28 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B14" t="n">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>What areas are within 3 minutes of driving time from the nearest fire station (from my current location) in Oleander</t>
+          <t>What areas are within a quarter mile of a restaurant in Gresham</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Gresham</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>amenity=restaurant</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
           <t>done</t>
@@ -1425,34 +1457,18 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Network analysis</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
@@ -1460,19 +1476,15 @@
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>어디로 부터 가장 가까운 소방서</t>
-        </is>
-      </c>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z14" t="n">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="AA14" t="b">
         <v>0</v>
@@ -1480,26 +1492,26 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B15" t="n">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>What areas are within 500 meters from religious places in Karbala in Iraq</t>
+          <t>What areas are within a quarter mile of a store in Gresham</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Karbala, Iraq</t>
+          <t>Gresham</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>landuse=religious</t>
+          <t>shop=*</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1533,7 +1545,11 @@
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>Shop이 너무나 많다</t>
+        </is>
+      </c>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr">
         <is>
@@ -1549,28 +1565,28 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B16" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>What areas are accessible within two miles of urban landuse in Loudoun County in US</t>
+          <t>What areas are within a quarter mile of light rail stop in Gresham</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Loudoun County</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
+          <t>Gresham</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>railway=tram_stop, light_rail</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr">
         <is>
           <t>done</t>
@@ -1578,24 +1594,20 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Buffer</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
@@ -1606,19 +1618,15 @@
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr">
-        <is>
-          <t>what area는 그냥 boundary만 얘기하는 것인가? 아니면 다른 attribute도 clip하라는 것인가. 일단 clip. Urban tag를 그렇게 사용하지도 않는다</t>
-        </is>
-      </c>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>data editing,data queries,buffer,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z16" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="AA16" t="b">
         <v>0</v>
@@ -1626,22 +1634,26 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B17" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>What areas have an monthly rainfall of more than 1000 millimeters in the Cape Peninsula</t>
+          <t>What areas are accessible within two miles of urban landuse in Loudoun County in US</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>Loudoun County</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
@@ -1651,29 +1663,25 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data editing</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Data model conversion</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
@@ -1683,15 +1691,19 @@
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>what area는 그냥 boundary만 얘기하는 것인가? 아니면 다른 attribute도 clip하라는 것인가. 일단 clip. Urban tag를 그렇게 사용하지도 않는다</t>
+        </is>
+      </c>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data editing,data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="Z17" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="AA17" t="b">
         <v>0</v>
@@ -1699,24 +1711,28 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B18" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>What areas have an annual amount of snowfall more than 1000 millimeters in the Cape Peninsula</t>
+          <t>What areas do have temperature in Celsius less than 0 degrees in Spain</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>the Cape Peninsula</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>monitoring:weather=yes</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr">
         <is>
           <t>done</t>
@@ -1772,14 +1788,14 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B19" t="n">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>What areas have slope larger than 15 percent and smaller than 60 percent in the Cape Peninsula</t>
+          <t>What areas have an monthly rainfall of more than 1000 millimeters in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1797,7 +1813,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Topography</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1833,11 +1849,11 @@
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
+          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z19" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AA19" t="b">
         <v>0</v>
@@ -1845,28 +1861,24 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B20" t="n">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>What houses are less than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
+          <t>What areas have slope larger than 15 percent and smaller than 60 percent in the Cape Peninsula</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>the Cape Peninsula</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>amenity=school, building=house</t>
-        </is>
-      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
           <t>done</t>
@@ -1874,27 +1886,27 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Topography</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>classification</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>buffer</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
+          <t>Data model conversion</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>Data queries</t>
         </is>
       </c>
       <c r="N20" t="inlineStr"/>
@@ -1910,11 +1922,11 @@
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
+          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="Z20" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="AA20" t="b">
         <v>0</v>
@@ -1922,14 +1934,14 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B21" t="n">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>What houses are for sale and within 1km from the nearest school (from my current location) in Utrecht</t>
+          <t>What houses are for sale and within 0.5km from the main roads in Utrecht</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1941,7 +1953,7 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>amenity=school, building=house</t>
+          <t>highway=motorway, building=house</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1951,29 +1963,25 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Buffer</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>buffer</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
@@ -1987,11 +1995,11 @@
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr">
         <is>
-          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
+          <t>data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z21" t="n">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="AA21" t="b">
         <v>0</v>
@@ -1999,14 +2007,14 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B22" t="n">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>What houses are for sale outside flood zone in Utrecht</t>
+          <t>Which houses are larger than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2018,7 +2026,7 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>boundary=urban, building=house</t>
+          <t>amenity=school, building=house</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -2028,21 +2036,29 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>network analysis</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
@@ -2052,19 +2068,15 @@
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
-        </is>
-      </c>
+      <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries</t>
+          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z22" t="n">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="AA22" t="b">
         <v>0</v>
@@ -2072,14 +2084,14 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B23" t="n">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>What houses are for sale in flood zone in Utrecht</t>
+          <t>What houses are less than 30 square meters and within 1km from the nearest school (from my current location) in Utrecht</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2091,7 +2103,7 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>boundary=urban, building=house</t>
+          <t>amenity=school, building=house</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2101,21 +2113,29 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>network analysis</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
@@ -2125,19 +2145,15 @@
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
-        </is>
-      </c>
+      <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data queries</t>
+          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z23" t="n">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="AA23" t="b">
         <v>0</v>
@@ -2145,14 +2161,14 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B24" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>What houses are larger than 30 square meters in urban areas in Utrecht</t>
+          <t>What houses are for sale in flood zone in Utrecht</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2218,26 +2234,26 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B25" t="n">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>What is weighted average coordinates of bank branches in Oleander</t>
+          <t>What houses are for sale in urban areas in Utrecht</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>amenity=bank</t>
+          <t>boundary=urban, building=house</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2252,12 +2268,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Generalization</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="L25" t="inlineStr"/>
@@ -2270,20 +2286,20 @@
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr">
-        <is>
-          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
-        </is>
-      </c>
-      <c r="W25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>osm urban이 있긴 하지만 거의 안쓴다</t>
+        </is>
+      </c>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
+          <t>data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z25" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA25" t="b">
         <v>0</v>
@@ -2291,28 +2307,24 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B26" t="n">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>What is the central feature of bank branches in Oleander</t>
+          <t>What is the average rating of street pavement for each borough in New York City</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>New York City</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>amenity=bank</t>
-        </is>
-      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
           <t>done</t>
@@ -2320,20 +2332,24 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Data editing</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Generalization</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr"/>
+          <t>Data editing</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
@@ -2343,20 +2359,16 @@
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr">
-        <is>
-          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
-        </is>
-      </c>
+      <c r="V26" t="inlineStr"/>
       <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
+          <t>data editing,overlay analysis,data editing,data queries</t>
         </is>
       </c>
       <c r="Z26" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="AA26" t="b">
         <v>0</v>
@@ -2364,28 +2376,28 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B27" t="n">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>What is the cervix cancer mortality rate of white females for each city in the Western USA from 1970 to 1994</t>
+          <t>Show me the central feature of bank branches in Oleander</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve">the Western USA </t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>from 1970 to 1994</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>amenity=bank</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
           <t>done</t>
@@ -2393,15 +2405,19 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr"/>
+          <t>Generalization</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
@@ -2412,16 +2428,20 @@
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
-      <c r="V27" t="inlineStr"/>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
+        </is>
+      </c>
       <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
         </is>
       </c>
       <c r="Z27" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="AA27" t="b">
         <v>0</v>
@@ -2429,24 +2449,28 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B28" t="n">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to green areas in Amsterdam</t>
+          <t>What is weighted average coordinates of bank branches in Oleander</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Amsterdam</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>amenity=bank</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
           <t>done</t>
@@ -2459,10 +2483,14 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
+          <t>Generalization</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
           <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
-      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
@@ -2473,16 +2501,20 @@
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
-      <c r="V28" t="inlineStr"/>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
+        </is>
+      </c>
       <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
         </is>
       </c>
       <c r="Z28" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="AA28" t="b">
         <v>0</v>
@@ -2490,28 +2522,24 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B29" t="n">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to hospitals in Oleander</t>
+          <t>What is the Euclidean distance to the rivers in Crook, Deschutes, and Jefferson county</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Crook, Deschutes, Jefferson county</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>amenity=hospital</t>
-        </is>
-      </c>
+      <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
           <t>done</t>
@@ -2555,28 +2583,24 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B30" t="n">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>What is the Euclidean distance to schools in Utrecht</t>
+          <t>What is the Euclidean distance to tram stations in Amsterdam</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Utrecht</t>
+          <t>Amsterdam</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>amenity=school</t>
-        </is>
-      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
           <t>done</t>
@@ -2685,28 +2709,28 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B32" t="n">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>What is the land use in Netherlands</t>
+          <t>What is the kernel density of traffic accidents in Pasadena, California</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>Pasadena</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>California</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>landuse=*</t>
-        </is>
-      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
           <t>done</t>
@@ -2717,7 +2741,11 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
@@ -2734,11 +2762,11 @@
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z32" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA32" t="b">
         <v>0</v>
@@ -2746,24 +2774,28 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B33" t="n">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>What is the literacy rate for each country in Africa</t>
+          <t>What is the land use in Netherlands</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>landuse=*</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr">
         <is>
           <t>done</t>
@@ -2771,14 +2803,10 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>data editing</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
@@ -2795,11 +2823,11 @@
       <c r="X33" t="inlineStr"/>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="Z33" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA33" t="b">
         <v>0</v>
@@ -2807,19 +2835,19 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B34" t="n">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>What is the mean center of customers weighted by the number of transactions in Oleander city</t>
+          <t>What is the literacy rate for each country in Africa</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Oleander city</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -2832,12 +2860,12 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
@@ -2856,11 +2884,11 @@
       <c r="X34" t="inlineStr"/>
       <c r="Y34" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="Z34" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AA34" t="b">
         <v>0</v>
@@ -2868,14 +2896,14 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B35" t="n">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>What is the mean center of the fire calls for each alarm territory in Fort Worth in 2017</t>
+          <t>What is the mean center of crimes weighted by the severity in Fort Worth</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2884,11 +2912,7 @@
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
@@ -2902,14 +2926,10 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
           <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
+      <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
@@ -2925,11 +2945,11 @@
       <c r="X35" t="inlineStr"/>
       <c r="Y35" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+          <t xml:space="preserve">data queries,geostatistics  </t>
         </is>
       </c>
       <c r="Z35" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="AA35" t="b">
         <v>0</v>
@@ -2937,27 +2957,27 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B36" t="n">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>What is the median population for each census block in Tarrant County in Texas</t>
+          <t>What is the mean center of the fire calls for each alarm territory in Fort Worth in 2017</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Tarrant County</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Texas</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr"/>
+          <t>Fort Worth</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
@@ -2966,7 +2986,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2976,14 +2996,10 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>data editing</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Geostatistics  </t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
@@ -2998,11 +3014,11 @@
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data editing,data queries</t>
+          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
         </is>
       </c>
       <c r="Z36" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="AA36" t="b">
         <v>0</v>
@@ -3010,22 +3026,26 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B37" t="n">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>What is the number of arson cases in Fort Worth on February 2004</t>
+          <t>What is the median population for each census block in Tarrant County in Texas</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Fort Worth on February 2004</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
+          <t>Tarrant County</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Texas</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
@@ -3040,11 +3060,19 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
@@ -3059,11 +3087,11 @@
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr">
         <is>
-          <t>data editing,data queries</t>
+          <t>data editing,overlay analysis,data editing,data queries</t>
         </is>
       </c>
       <c r="Z37" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="AA37" t="b">
         <v>0</v>
@@ -3071,23 +3099,27 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B38" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>What is the number of buildings within 3 minutes of driving time from fire stations in Oleander</t>
+          <t>What is the number of crime cases for each police district in Texas in 2018</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
@@ -3096,17 +3128,17 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3114,16 +3146,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
@@ -3136,11 +3160,11 @@
       <c r="X38" t="inlineStr"/>
       <c r="Y38" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+          <t>data editing,data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z38" t="n">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="AA38" t="b">
         <v>0</v>
@@ -3148,14 +3172,14 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B39" t="n">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>What is the number of high school students for each senior high school district in Oleander</t>
+          <t>What is the number of dwelling units inside the flood zones in Oleander</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3173,24 +3197,20 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>data editing</t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
@@ -3205,11 +3225,11 @@
       <c r="X39" t="inlineStr"/>
       <c r="Y39" t="inlineStr">
         <is>
-          <t>data editing,data queries,overlay analysis,data queries</t>
+          <t>data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z39" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="AA39" t="b">
         <v>0</v>
@@ -3217,26 +3237,22 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B40" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>What is the number of Hispanics for each census block in Tarrant County in Texas</t>
+          <t>What is the number of high school students for each senior high school district in Oleander</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Tarrant County</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Texas</t>
-        </is>
-      </c>
+          <t>Oleander</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -3290,27 +3306,23 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B41" t="n">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">What is the number of injured pedestrians for each census tract in Georgia from 2000 to 2007 </t>
+          <t>What is the point density of fire calls in Oleander</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> from 2000 to 2007 </t>
-        </is>
-      </c>
+      <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
@@ -3324,17 +3336,17 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
           <t>Overlay analysis</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>data editing</t>
-        </is>
-      </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t xml:space="preserve">Geostatistics  </t>
         </is>
       </c>
       <c r="M41" t="inlineStr"/>
@@ -3351,11 +3363,11 @@
       <c r="X41" t="inlineStr"/>
       <c r="Y41" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data editing,data queries</t>
+          <t xml:space="preserve">data editing,data queries,overlay analysis,geostatistics  </t>
         </is>
       </c>
       <c r="Z41" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AA41" t="b">
         <v>0</v>
@@ -3363,23 +3375,27 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B42" t="n">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>What is the number of luxury hotels in Happy Valley ski resort</t>
+          <t>What is the tornado path in Oleander in April 2011</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Happy Valley ski resort</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>April 2011</t>
+        </is>
+      </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
@@ -3388,10 +3404,14 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr"/>
+          <t>data editing</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
@@ -3408,11 +3428,11 @@
       <c r="X42" t="inlineStr"/>
       <c r="Y42" t="inlineStr">
         <is>
-          <t>data queries</t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="Z42" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA42" t="b">
         <v>0</v>
@@ -3420,24 +3440,28 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B43" t="n">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>What is the point density of fire calls in Oleander</t>
+          <t>What is the total area of agriculture in Netherlands</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>agriculture=*, landuse=argiculture</t>
+        </is>
+      </c>
       <c r="H43" t="inlineStr">
         <is>
           <t>done</t>
@@ -3445,22 +3469,22 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Geometry measurement</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
           <t>data editing</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Geostatistics  </t>
+          <t>Data queries</t>
         </is>
       </c>
       <c r="M43" t="inlineStr"/>
@@ -3477,11 +3501,11 @@
       <c r="X43" t="inlineStr"/>
       <c r="Y43" t="inlineStr">
         <is>
-          <t xml:space="preserve">data editing,data queries,overlay analysis,geostatistics  </t>
+          <t>data queries,geometry measurement,data editing,data queries</t>
         </is>
       </c>
       <c r="Z43" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA43" t="b">
         <v>0</v>
@@ -3489,26 +3513,30 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B44" t="n">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>What is the total area of agriculture in Netherlands</t>
+          <t>What is the total population for each census block in Tarrant County, Texas</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>Tarrant County</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Texas</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>agriculture=*, landuse=argiculture</t>
+          <t>population</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3518,24 +3546,16 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Data queries</t>
+          <t>data editing</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>data editing</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr"/>
@@ -3550,11 +3570,11 @@
       <c r="X44" t="inlineStr"/>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data editing,data queries</t>
+          <t>data editing,data queries</t>
         </is>
       </c>
       <c r="Z44" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="AA44" t="b">
         <v>0</v>
@@ -3562,24 +3582,28 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B45" t="n">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>What is the total population within a four-minute travel time from fire stations in Poway</t>
+          <t>What liquor stores are within 1000 foot of parks in El Cajon</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Poway</t>
+          <t>El Cajon</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>shop=alcohol, leisure=park</t>
+        </is>
+      </c>
       <c r="H45" t="inlineStr">
         <is>
           <t>done</t>
@@ -3592,12 +3616,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Network analysis</t>
+          <t>buffer</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Overlay analysis</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3605,16 +3629,8 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
@@ -3627,11 +3643,11 @@
       <c r="X45" t="inlineStr"/>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
+          <t>data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z45" t="n">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="AA45" t="b">
         <v>0</v>
@@ -3639,26 +3655,26 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B46" t="n">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>What liquor stores are within 1000 foot of parks in El Cajon</t>
+          <t>Where are forestry lands in Happy Valley ski resort</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>El Cajon</t>
+          <t>Happy Valley ski resort</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
-          <t>shop=alcohol, leisure=park</t>
+          <t>Tag:landuse=forestry</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3671,21 +3687,9 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>buffer</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
@@ -3700,11 +3704,11 @@
       <c r="X46" t="inlineStr"/>
       <c r="Y46" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="Z46" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AA46" t="b">
         <v>0</v>
@@ -3712,26 +3716,26 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B47" t="n">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>What liquor stores are within 1000 foot of schools in El Cajon</t>
+          <t>Where are the commercial areas in Amsterdam</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>El Cajon</t>
+          <t>Amsterdam</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>shop=alcohol, amenity=school</t>
+          <t>landuse=commercial</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3746,19 +3750,15 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>buffer</t>
+          <t>Geometry measurement</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr"/>
@@ -3773,11 +3773,11 @@
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries</t>
+          <t>data queries,geometry measurement,data queries</t>
         </is>
       </c>
       <c r="Z47" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AA47" t="b">
         <v>0</v>
@@ -3785,30 +3785,26 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B48" t="n">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Where are not protected region in Assam in India</t>
+          <t>Where are the industrial areas in Utrecht</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>landuse=conservation</t>
+          <t>landuse=industrial</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3858,26 +3854,26 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B49" t="n">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Where are the commercial areas in Amsterdam</t>
+          <t>Where are the luxury hotels with more than 20 bedrooms in Happy Valley ski resort</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Amsterdam</t>
+          <t>Happy Valley ski resort</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>landuse=commercial</t>
+          <t>beds=*, tourism=hotel</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3927,24 +3923,28 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B50" t="n">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Where are the five star hotels in the Happy Valley ski resort</t>
+          <t>Which houses are within 2 minutes driving time from fire stations  (from my current location) in Oleander</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>the Happy Valley ski resort</t>
+          <t>Oleander</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>amenity=fire_station</t>
+        </is>
+      </c>
       <c r="H50" t="inlineStr">
         <is>
           <t>done</t>
@@ -3957,16 +3957,24 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Geometry measurement</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
@@ -3980,11 +3988,11 @@
       <c r="X50" t="inlineStr"/>
       <c r="Y50" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="Z50" t="n">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="AA50" t="b">
         <v>0</v>
@@ -3992,26 +4000,26 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B51" t="n">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Which houses are within 2 minutes driving time from fire stations  (from my current location) in Oleander</t>
+          <t>Which houses have construction year between 1990 and 2000 in Utrecht</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Oleander</t>
+          <t>Utrecht</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
-          <t>amenity=fire_station</t>
+          <t>year_of_construction=*</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4024,26 +4032,10 @@
           <t>Data queries</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Network analysis</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>classification</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>Overlay analysis</t>
-        </is>
-      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
@@ -4057,11 +4049,11 @@
       <c r="X51" t="inlineStr"/>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>data queries</t>
         </is>
       </c>
       <c r="Z51" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="AA51" t="b">
         <v>0</v>
@@ -4219,26 +4211,26 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B54" t="n">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Which proposed wind farm are nearest to the high way in Scotland</t>
+          <t>Which schools are not within 3 minutes of driving time from a fire station in Fort Worth</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Scotland</t>
+          <t>Fort Worth</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
-          <t>highway=*</t>
+          <t>amenity=fire_station, amenity=school</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -4253,17 +4245,29 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>network analysis</t>
+          <t>Network analysis</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Data queries</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Data queries</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Overlay analysis</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>data queries</t>
+        </is>
+      </c>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
@@ -4276,11 +4280,11 @@
       <c r="X54" t="inlineStr"/>
       <c r="Y54" t="inlineStr">
         <is>
-          <t>data queries,network analysis,data queries</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="Z54" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="AA54" t="b">
         <v>0</v>
@@ -4288,14 +4292,14 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B55" t="n">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Which wind farm proposals are nearest to the high way in Scotland</t>
+          <t>Which proposed wind farm are nearest to the high way in Scotland</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">

</xml_diff>